<commit_message>
Currently working through all the simulations to get good results.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons_rev2.xlsx
+++ b/metaboliccostcomparisons_rev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71AB045-63C7-42E2-8826-CF41A0D9D72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DEBF78-4DEB-43CA-9F9A-9BA95E48266A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="alldata_1step" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="118">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -388,6 +389,9 @@
   </si>
   <si>
     <t>MSE without basal</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -3854,10 +3858,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8.9249700000000001</c:v>
+                  <c:v>9.9407420000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9254034999999998</c:v>
+                  <c:v>11.02410725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3902,10 +3906,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.0244367499999996</c:v>
+                  <c:v>10.679057500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1095760000000006</c:v>
+                  <c:v>9.9984134999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3950,10 +3954,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>13.055065750000001</c:v>
+                  <c:v>13.6868935</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6310232500000001</c:v>
+                  <c:v>10.661610250000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3998,10 +4002,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.6294970000000006</c:v>
+                  <c:v>11.8646075</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.581848749999999</c:v>
+                  <c:v>11.5270335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4046,10 +4050,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.7281172500000004</c:v>
+                  <c:v>11.077177250000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.27927375</c:v>
+                  <c:v>11.60830275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4094,10 +4098,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.739731750000001</c:v>
+                  <c:v>11.219330250000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.91831575</c:v>
+                  <c:v>12.991008249999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4135,6 +4139,21 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -5034,10 +5053,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.7249699999999999</c:v>
+                  <c:v>8.7407420000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7254035000000005</c:v>
+                  <c:v>9.8241072500000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5082,10 +5101,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.8244367499999994</c:v>
+                  <c:v>9.4790575000000015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9095760000000004</c:v>
+                  <c:v>8.7984135000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5130,10 +5149,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.855065750000001</c:v>
+                  <c:v>12.486893500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4310232500000009</c:v>
+                  <c:v>9.4616102500000014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5178,10 +5197,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8.4294970000000013</c:v>
+                  <c:v>10.664607500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3818487499999996</c:v>
+                  <c:v>10.327033500000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5226,10 +5245,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8.5281172500000011</c:v>
+                  <c:v>9.8771772500000026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0792737500000005</c:v>
+                  <c:v>10.408302750000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5274,10 +5293,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.5397317500000014</c:v>
+                  <c:v>10.019330250000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.71831575</c:v>
+                  <c:v>11.791008249999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5931,6 +5950,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Experimental</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="4472C4"/>
@@ -5941,41 +5963,44 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="9"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>7</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>9</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>10</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>11</c:v>
-              </c:pt>
+            <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                  </c15:fullRef>
                 </c:ext>
               </c:extLst>
-            </c:strLit>
+              <c:f>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -5986,10 +6011,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(alldata_1step!$M$3:$M$4,alldata_1step!$M$6:$M$12)</c:f>
+              <c:f>(alldata_1step!$M$3:$M$4,alldata_1step!$M$6:$M$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>-4.4476325130031995</c:v>
                 </c:pt>
@@ -6026,6 +6051,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Simulated</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="ED7D31"/>
@@ -6036,41 +6064,44 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="9"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>7</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>9</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>10</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>11</c:v>
-              </c:pt>
+            <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                  </c15:fullRef>
                 </c:ext>
               </c:extLst>
-            </c:strLit>
+              <c:f>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -6092,22 +6123,22 @@
                   <c:v>-3.7297543833232742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-11.46575628278968</c:v>
+                  <c:v>-11.027620346876809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.0764072562170335</c:v>
+                  <c:v>7.7359855842192555</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.612419139041045</c:v>
+                  <c:v>31.974295812914072</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-10.151003020593338</c:v>
+                  <c:v>3.2688380453108823</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6.0704910456081285</c:v>
+                  <c:v>-5.1029021038036015</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-10.995981341564779</c:v>
+                  <c:v>-15.02567009059635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6186,6 +6217,51 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
@@ -6265,6 +6341,51 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
@@ -6673,22 +6794,22 @@
                   <c:v>-6.1489278867575043</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-11.46575628278968</c:v>
+                  <c:v>-11.027620346876809</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.0764072562170335</c:v>
+                  <c:v>7.7359855842192555</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.612419139041045</c:v>
+                  <c:v>31.974295812914072</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-10.151003020593338</c:v>
+                  <c:v>3.2688380453108823</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6.0704910456081285</c:v>
+                  <c:v>-5.1029021038036015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-10.995981341564779</c:v>
+                  <c:v>-15.02567009059635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6971,22 +7092,22 @@
                   <c:v>-0.64127275000000061</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0004334999999998</c:v>
+                  <c:v>-1.0833652499999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-8.5139250000000999E-2</c:v>
+                  <c:v>0.68064400000000091</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4240425000000005</c:v>
+                  <c:v>3.0252832499999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.95235174999999828</c:v>
+                  <c:v>0.33757400000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.55115649999999938</c:v>
+                  <c:v>-0.53112549999999814</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.178583999999999</c:v>
+                  <c:v>-1.7716779999999979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7161,22 +7282,22 @@
                   <c:v>-0.64127275000000061</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0004335000000006</c:v>
+                  <c:v>-1.0833652499999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-8.5139250000000999E-2</c:v>
+                  <c:v>0.68064400000000091</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4240425000000005</c:v>
+                  <c:v>3.0252832499999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.95235174999999828</c:v>
+                  <c:v>0.33757400000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.55115649999999938</c:v>
+                  <c:v>-0.53112549999999814</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.178583999999999</c:v>
+                  <c:v>-1.7716779999999979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8156,8 +8277,8 @@
       <xdr:rowOff>108136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>431019</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330166</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>51075</xdr:rowOff>
     </xdr:to>
@@ -8192,8 +8313,8 @@
       <xdr:rowOff>76568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>204359</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>1661125</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>111635</xdr:rowOff>
     </xdr:to>
@@ -8229,7 +8350,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>179411</xdr:colOff>
+      <xdr:colOff>179412</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>12006</xdr:rowOff>
     </xdr:to>
@@ -13789,8 +13910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BR81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q94" sqref="Q94"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13808,12 +13929,12 @@
     <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44" customWidth="1"/>
+    <col min="14" max="14" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="29.140625" customWidth="1"/>
-    <col min="17" max="17" width="43.7109375" customWidth="1"/>
+    <col min="17" max="17" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.7109375" customWidth="1"/>
+    <col min="37" max="37" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13.140625" customWidth="1"/>
     <col min="39" max="39" width="13.28515625" customWidth="1"/>
     <col min="40" max="40" width="21" bestFit="1" customWidth="1"/>
@@ -13877,6 +13998,9 @@
       <c r="Q1" t="s">
         <v>113</v>
       </c>
+      <c r="R1" t="s">
+        <v>117</v>
+      </c>
       <c r="AF1" t="s">
         <v>85</v>
       </c>
@@ -13971,6 +14095,9 @@
         <f>(K2-K3)/K3*100</f>
         <v>-10.753270260491925</v>
       </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
       <c r="AH2" t="s">
         <v>14</v>
       </c>
@@ -14071,6 +14198,9 @@
         <f>(K4-K5)/K5*100</f>
         <v>-8.0372380116609783</v>
       </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
       <c r="AG3">
         <v>0</v>
       </c>
@@ -14228,6 +14358,9 @@
         <f>(K6-K7)/K7*100</f>
         <v>-3.7297543833232742</v>
       </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
       <c r="AG4">
         <v>1</v>
       </c>
@@ -14371,6 +14504,9 @@
         <f>(K8-K9)/K9*100</f>
         <v>-6.1489278867575043</v>
       </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
       <c r="AG5">
         <v>2</v>
       </c>
@@ -14505,13 +14641,16 @@
       </c>
       <c r="N6">
         <f>(J10-J11)/J10*100</f>
-        <v>-11.209376614151081</v>
+        <v>-10.898233250596382</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6">
         <f>(K10-K11)/K11*100</f>
-        <v>-11.46575628278968</v>
+        <v>-11.027620346876809</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
       </c>
       <c r="AG6">
         <v>3</v>
@@ -14614,13 +14753,16 @@
       </c>
       <c r="N7">
         <f>(J12-J13)/J12*100</f>
-        <v>-0.94343007058031636</v>
+        <v>6.3736336282485677</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7">
         <f>(K12-K13)/K13*100</f>
-        <v>-1.0764072562170335</v>
+        <v>7.7359855842192555</v>
+      </c>
+      <c r="R7">
+        <v>7</v>
       </c>
       <c r="AG7">
         <v>8</v>
@@ -14757,13 +14899,16 @@
       </c>
       <c r="N8">
         <f>(J14-J15)/J14*100</f>
-        <v>26.227692495535692</v>
+        <v>22.103505444825732</v>
       </c>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8">
         <f>(K14-K15)/K15*100</f>
-        <v>40.612419139041045</v>
+        <v>31.974295812914072</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
       </c>
       <c r="AG8">
         <v>9</v>
@@ -14888,13 +15033,16 @@
       </c>
       <c r="N9">
         <f>(J16-J17)/J16*100</f>
-        <v>-9.8899428495589987</v>
+        <v>2.8452184364295241</v>
       </c>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9">
         <f>(K16-K17)/K17*100</f>
-        <v>-10.151003020593338</v>
+        <v>3.2688380453108823</v>
+      </c>
+      <c r="R9">
+        <v>9</v>
       </c>
       <c r="AG9">
         <v>10</v>
@@ -15011,11 +15159,11 @@
       </c>
       <c r="J10">
         <f>F34</f>
-        <v>8.9249700000000001</v>
+        <v>9.9407420000000002</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>7.7249699999999999</v>
+        <v>8.7407420000000009</v>
       </c>
       <c r="L10">
         <v>5</v>
@@ -15026,13 +15174,16 @@
       </c>
       <c r="N10">
         <f>(J18-J19)/J18*100</f>
-        <v>-5.6656029716335849</v>
+        <v>-4.7947729643849302</v>
       </c>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10">
         <f>(K18-K19)/K19*100</f>
-        <v>-6.0704910456081285</v>
+        <v>-5.1029021038036015</v>
+      </c>
+      <c r="R10">
+        <v>10</v>
       </c>
       <c r="AG10">
         <v>11</v>
@@ -15117,11 +15268,11 @@
       </c>
       <c r="J11">
         <f>F38</f>
-        <v>9.9254034999999998</v>
+        <v>11.02410725</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>8.7254035000000005</v>
+        <v>9.8241072500000008</v>
       </c>
       <c r="L11">
         <v>5</v>
@@ -15132,13 +15283,16 @@
       </c>
       <c r="N11">
         <f>(J20-J21)/J20*100</f>
-        <v>-10.974054356618348</v>
+        <v>-15.791299128573186</v>
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11">
         <f>(K20-K21)/K21*100</f>
-        <v>-10.995981341564779</v>
+        <v>-15.02567009059635</v>
+      </c>
+      <c r="R11">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:70" x14ac:dyDescent="0.25">
@@ -15163,11 +15317,11 @@
       </c>
       <c r="J12">
         <f>F42</f>
-        <v>9.0244367499999996</v>
+        <v>10.679057500000001</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>7.8244367499999994</v>
+        <v>9.4790575000000015</v>
       </c>
       <c r="L12">
         <v>7</v>
@@ -15200,11 +15354,11 @@
       </c>
       <c r="J13">
         <f>F46</f>
-        <v>9.1095760000000006</v>
+        <v>9.9984134999999998</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>7.9095760000000004</v>
+        <v>8.7984135000000006</v>
       </c>
       <c r="L13">
         <v>7</v>
@@ -15242,11 +15396,11 @@
       </c>
       <c r="J14">
         <f>F50</f>
-        <v>13.055065750000001</v>
+        <v>13.6868935</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>11.855065750000001</v>
+        <v>12.486893500000001</v>
       </c>
       <c r="L14">
         <v>8</v>
@@ -15283,11 +15437,11 @@
       </c>
       <c r="J15">
         <f>F54</f>
-        <v>9.6310232500000001</v>
+        <v>10.661610250000001</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>8.4310232500000009</v>
+        <v>9.4616102500000014</v>
       </c>
       <c r="L15">
         <v>8</v>
@@ -15317,11 +15471,11 @@
       </c>
       <c r="J16">
         <f>F58</f>
-        <v>9.6294970000000006</v>
+        <v>11.8646075</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>8.4294970000000013</v>
+        <v>10.664607500000001</v>
       </c>
       <c r="L16">
         <v>9</v>
@@ -15351,11 +15505,11 @@
       </c>
       <c r="J17">
         <f>F62</f>
-        <v>10.581848749999999</v>
+        <v>11.5270335</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>9.3818487499999996</v>
+        <v>10.327033500000001</v>
       </c>
       <c r="L17">
         <v>9</v>
@@ -15389,11 +15543,11 @@
       </c>
       <c r="J18">
         <f>F66</f>
-        <v>9.7281172500000004</v>
+        <v>11.077177250000002</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>8.5281172500000011</v>
+        <v>9.8771772500000026</v>
       </c>
       <c r="L18">
         <v>10</v>
@@ -15423,11 +15577,11 @@
       </c>
       <c r="J19">
         <f>F70</f>
-        <v>10.27927375</v>
+        <v>11.60830275</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>9.0792737500000005</v>
+        <v>10.408302750000001</v>
       </c>
       <c r="L19">
         <v>10</v>
@@ -15457,11 +15611,11 @@
       </c>
       <c r="J20">
         <f>F74</f>
-        <v>10.739731750000001</v>
+        <v>11.219330250000001</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>9.5397317500000014</v>
+        <v>10.019330250000001</v>
       </c>
       <c r="L20">
         <v>13</v>
@@ -15491,11 +15645,11 @@
       </c>
       <c r="J21">
         <f>F78</f>
-        <v>11.91831575</v>
+        <v>12.991008249999998</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>10.71831575</v>
+        <v>11.791008249999999</v>
       </c>
       <c r="L21">
         <v>13</v>
@@ -15679,7 +15833,7 @@
       </c>
       <c r="I30">
         <f>AVERAGE(J30:J49)</f>
-        <v>1.9750345489298506</v>
+        <v>2.3566705198385196</v>
       </c>
       <c r="J30">
         <f>(J2-I2)^2</f>
@@ -15687,7 +15841,7 @@
       </c>
       <c r="K30">
         <f>AVERAGE(L30:L49)</f>
-        <v>2.5612753489298496</v>
+        <v>1.2951884398385187</v>
       </c>
       <c r="L30">
         <f>(K2-I2)^2</f>
@@ -15819,11 +15973,11 @@
         <v>34</v>
       </c>
       <c r="E34">
-        <v>8.5934810000000006</v>
+        <v>9.7181440000000006</v>
       </c>
       <c r="F34">
         <f>AVERAGE(E34:E37)</f>
-        <v>8.9249700000000001</v>
+        <v>9.9407420000000002</v>
       </c>
       <c r="G34">
         <v>9.4284049999999997</v>
@@ -15842,11 +15996,11 @@
       </c>
       <c r="O34">
         <f>J10-J11</f>
-        <v>-1.0004334999999998</v>
+        <v>-1.0833652499999999</v>
       </c>
       <c r="P34">
         <f>K10-K11</f>
-        <v>-1.0004335000000006</v>
+        <v>-1.0833652499999999</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
@@ -15860,7 +16014,7 @@
         <v>37</v>
       </c>
       <c r="E35">
-        <v>8.8216180000000008</v>
+        <v>9.7003730000000008</v>
       </c>
       <c r="G35">
         <v>9.4284049999999997</v>
@@ -15879,11 +16033,11 @@
       </c>
       <c r="O35">
         <f>J12-J13</f>
-        <v>-8.5139250000000999E-2</v>
+        <v>0.68064400000000091</v>
       </c>
       <c r="P35">
         <f>K12-K13</f>
-        <v>-8.5139250000000999E-2</v>
+        <v>0.68064400000000091</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
@@ -15897,7 +16051,7 @@
         <v>38</v>
       </c>
       <c r="E36">
-        <v>9.0670350000000006</v>
+        <v>10.118931</v>
       </c>
       <c r="G36">
         <v>9.4284049999999997</v>
@@ -15916,11 +16070,11 @@
       </c>
       <c r="O36">
         <f>J14-J15</f>
-        <v>3.4240425000000005</v>
+        <v>3.0252832499999993</v>
       </c>
       <c r="P36">
         <f>K14-K15</f>
-        <v>3.4240425000000005</v>
+        <v>3.0252832499999993</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
@@ -15934,7 +16088,7 @@
         <v>39</v>
       </c>
       <c r="E37">
-        <v>9.217746</v>
+        <v>10.225519999999999</v>
       </c>
       <c r="G37">
         <v>9.4284049999999997</v>
@@ -15953,11 +16107,11 @@
       </c>
       <c r="O37">
         <f>J16-J17</f>
-        <v>-0.95235174999999828</v>
+        <v>0.33757400000000004</v>
       </c>
       <c r="P37">
         <f>K16-K17</f>
-        <v>-0.95235174999999828</v>
+        <v>0.33757400000000004</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -15971,22 +16125,22 @@
         <v>34</v>
       </c>
       <c r="E38">
-        <v>10.541696</v>
+        <v>11.057202</v>
       </c>
       <c r="F38">
         <f>AVERAGE(E38:E41)</f>
-        <v>9.9254034999999998</v>
+        <v>11.02410725</v>
       </c>
       <c r="G38">
         <v>10.921894999999999</v>
       </c>
       <c r="J38">
         <f t="shared" si="1"/>
-        <v>0.25344679922499963</v>
+        <v>0.26248920156900052</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
-        <v>2.9016907992249994</v>
+        <v>0.47288040156899835</v>
       </c>
       <c r="N38" s="14">
         <f>I18-I19</f>
@@ -15994,11 +16148,11 @@
       </c>
       <c r="O38">
         <f>J18-J19</f>
-        <v>-0.55115649999999938</v>
+        <v>-0.53112549999999814</v>
       </c>
       <c r="P38">
         <f>K18-K19</f>
-        <v>-0.55115649999999938</v>
+        <v>-0.53112549999999814</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
@@ -16012,18 +16166,18 @@
         <v>37</v>
       </c>
       <c r="E39">
-        <v>9.8150580000000005</v>
+        <v>10.943826</v>
       </c>
       <c r="G39">
         <v>10.921894999999999</v>
       </c>
       <c r="J39">
         <f t="shared" si="1"/>
-        <v>0.9929953095722488</v>
+        <v>1.0447344050062682E-2</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
-        <v>4.8245749095722443</v>
+        <v>1.2051379440500589</v>
       </c>
       <c r="N39" s="14">
         <f>I20-I21</f>
@@ -16031,11 +16185,11 @@
       </c>
       <c r="O39">
         <f>J20-J21</f>
-        <v>-1.178583999999999</v>
+        <v>-1.7716779999999979</v>
       </c>
       <c r="P39">
         <f>K20-K21</f>
-        <v>-1.178583999999999</v>
+        <v>-1.7716779999999979</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
@@ -16049,18 +16203,18 @@
         <v>38</v>
       </c>
       <c r="E40">
-        <v>9.6736260000000005</v>
+        <v>10.924265</v>
       </c>
       <c r="G40">
         <v>10.921894999999999</v>
       </c>
       <c r="J40">
         <f t="shared" si="1"/>
-        <v>0.12770563356056253</v>
+        <v>1.6828873993822531</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
-        <v>2.4253678335605633</v>
+        <v>9.4597993822503664E-3</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
@@ -16074,18 +16228,18 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <v>9.6712340000000001</v>
+        <v>11.171136000000001</v>
       </c>
       <c r="G41">
         <v>10.921894999999999</v>
       </c>
       <c r="J41">
         <f t="shared" si="1"/>
-        <v>0.18697927292100008</v>
+        <v>0.20832514990224926</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
-        <v>2.6647656729210007</v>
+        <v>0.55290154990225016</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -16099,22 +16253,22 @@
         <v>34</v>
       </c>
       <c r="E42">
-        <v>8.9168299999999991</v>
+        <v>10.75526</v>
       </c>
       <c r="F42">
         <f>AVERAGE(E42:E45)</f>
-        <v>9.0244367499999996</v>
+        <v>10.679057500000001</v>
       </c>
       <c r="G42">
         <v>9.3817959999999996</v>
       </c>
       <c r="J42">
         <f>(J14-I14)^2</f>
-        <v>13.685284756087567</v>
+        <v>18.759211147290248</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
-        <v>6.2468141560875692</v>
+        <v>9.8043539472902541</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
@@ -16128,18 +16282,18 @@
         <v>37</v>
       </c>
       <c r="E43">
-        <v>8.4183760000000003</v>
+        <v>10.262174</v>
       </c>
       <c r="G43">
         <v>9.3817959999999996</v>
       </c>
       <c r="J43">
         <f>(J15-I15)^2</f>
-        <v>0.4310864628980618</v>
+        <v>0.13988740723256335</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
-        <v>3.446858662898058</v>
+        <v>0.68225080723255949</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
@@ -16153,18 +16307,18 @@
         <v>38</v>
       </c>
       <c r="E44">
-        <v>9.6063010000000002</v>
+        <v>10.728984000000001</v>
       </c>
       <c r="G44">
         <v>9.3817959999999996</v>
       </c>
       <c r="J44">
         <f t="shared" ref="J44:J49" si="3">(J16-I16)^2</f>
-        <v>3.476024648099945E-2</v>
+        <v>4.1970467202302535</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
-        <v>1.9222186464809938</v>
+        <v>0.72023992023025263</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -16178,18 +16332,18 @@
         <v>39</v>
       </c>
       <c r="E45">
-        <v>9.1562400000000004</v>
+        <v>10.969811999999999</v>
       </c>
       <c r="G45">
         <v>9.3817959999999996</v>
       </c>
       <c r="J45">
         <f t="shared" si="3"/>
-        <v>0.27854882561756411</v>
+        <v>0.17422902105624957</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
-        <v>2.9852142256175656</v>
+        <v>0.61245102105624971</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -16203,22 +16357,22 @@
         <v>34</v>
       </c>
       <c r="E46">
-        <v>8.8664000000000005</v>
+        <v>9.8622639999999997</v>
       </c>
       <c r="F46">
         <f>AVERAGE(E46:E49)</f>
-        <v>9.1095760000000006</v>
+        <v>9.9984134999999998</v>
       </c>
       <c r="G46">
         <v>9.5419870000000007</v>
       </c>
       <c r="J46">
         <f t="shared" si="3"/>
-        <v>2.3261275146425628</v>
+        <v>3.1012882972562002E-2</v>
       </c>
       <c r="L46">
         <f t="shared" si="2"/>
-        <v>7.4265229146425593</v>
+        <v>1.8936642829725567</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
@@ -16232,18 +16386,18 @@
         <v>37</v>
       </c>
       <c r="E47">
-        <v>9.1042640000000006</v>
+        <v>10.020934</v>
       </c>
       <c r="G47">
         <v>9.5419870000000007</v>
       </c>
       <c r="J47">
         <f t="shared" si="3"/>
-        <v>4.0714411728515643</v>
+        <v>0.47437966188006292</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
-        <v>10.354116172851562</v>
+        <v>3.5673850618800609</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
@@ -16257,18 +16411,18 @@
         <v>38</v>
       </c>
       <c r="E48">
-        <v>9.2590160000000008</v>
+        <v>10.009589999999999</v>
       </c>
       <c r="G48">
         <v>9.5419870000000007</v>
       </c>
       <c r="J48">
         <f t="shared" si="3"/>
-        <v>0.38702800639806345</v>
+        <v>1.2137742886530638</v>
       </c>
       <c r="L48">
         <f t="shared" si="2"/>
-        <v>0.33395020639806083</v>
+        <v>9.6600886530622508E-3</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
@@ -16282,18 +16436,18 @@
         <v>39</v>
       </c>
       <c r="E49">
-        <v>9.2086240000000004</v>
+        <v>10.100866</v>
       </c>
       <c r="G49">
         <v>9.5419870000000007</v>
       </c>
       <c r="J49">
         <f t="shared" si="3"/>
-        <v>0.96157586970006181</v>
+        <v>4.2160090639100556</v>
       </c>
       <c r="L49">
         <f t="shared" si="2"/>
-        <v>4.8136469700062336E-2</v>
+        <v>0.72810766391006099</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
@@ -16307,11 +16461,11 @@
         <v>34</v>
       </c>
       <c r="E50">
-        <v>8.3306170000000002</v>
+        <v>9.1451019999999996</v>
       </c>
       <c r="F50">
         <f>AVERAGE(E50:E53)</f>
-        <v>13.055065750000001</v>
+        <v>13.6868935</v>
       </c>
       <c r="G50">
         <v>9.3557030000000001</v>
@@ -16328,7 +16482,7 @@
         <v>37</v>
       </c>
       <c r="E51">
-        <v>8.6614710000000006</v>
+        <v>9.7850619999999999</v>
       </c>
       <c r="G51">
         <v>9.3557030000000001</v>
@@ -16345,7 +16499,7 @@
         <v>38</v>
       </c>
       <c r="E52">
-        <v>17.156562000000001</v>
+        <v>18.428795000000001</v>
       </c>
       <c r="G52">
         <v>9.3557030000000001</v>
@@ -16362,7 +16516,7 @@
         <v>39</v>
       </c>
       <c r="E53">
-        <v>18.071612999999999</v>
+        <v>17.388615000000001</v>
       </c>
       <c r="G53">
         <v>9.3557030000000001</v>
@@ -16379,11 +16533,11 @@
         <v>34</v>
       </c>
       <c r="E54">
-        <v>9.7113940000000003</v>
+        <v>10.745618</v>
       </c>
       <c r="F54">
         <f>AVERAGE(E54:E57)</f>
-        <v>9.6310232500000001</v>
+        <v>10.661610250000001</v>
       </c>
       <c r="G54">
         <v>10.287595</v>
@@ -16400,7 +16554,7 @@
         <v>37</v>
       </c>
       <c r="E55">
-        <v>9.3742979999999996</v>
+        <v>10.12487</v>
       </c>
       <c r="G55">
         <v>10.287595</v>
@@ -16417,7 +16571,7 @@
         <v>38</v>
       </c>
       <c r="E56">
-        <v>9.9144349999999992</v>
+        <v>11.157829</v>
       </c>
       <c r="G56">
         <v>10.287595</v>
@@ -16434,7 +16588,7 @@
         <v>39</v>
       </c>
       <c r="E57">
-        <v>9.5239659999999997</v>
+        <v>10.618124</v>
       </c>
       <c r="G57">
         <v>10.287595</v>
@@ -16451,11 +16605,11 @@
         <v>34</v>
       </c>
       <c r="E58">
-        <v>9.3780129999999993</v>
+        <v>10.987154</v>
       </c>
       <c r="F58">
         <f>AVERAGE(E58:E61)</f>
-        <v>9.6294970000000006</v>
+        <v>11.8646075</v>
       </c>
       <c r="G58">
         <v>9.8159379999999992</v>
@@ -16472,7 +16626,7 @@
         <v>37</v>
       </c>
       <c r="E59">
-        <v>9.3205600000000004</v>
+        <v>14.224887000000001</v>
       </c>
       <c r="G59">
         <v>9.8159379999999992</v>
@@ -16489,7 +16643,7 @@
         <v>38</v>
       </c>
       <c r="E60">
-        <v>10.022251000000001</v>
+        <v>11.454666</v>
       </c>
       <c r="G60">
         <v>9.8159379999999992</v>
@@ -16506,7 +16660,7 @@
         <v>39</v>
       </c>
       <c r="E61">
-        <v>9.7971640000000004</v>
+        <v>10.791722999999999</v>
       </c>
       <c r="G61">
         <v>9.8159379999999992</v>
@@ -16523,11 +16677,11 @@
         <v>34</v>
       </c>
       <c r="E62">
-        <v>10.804575</v>
+        <v>11.754167000000001</v>
       </c>
       <c r="F62">
         <f>AVERAGE(E62:E65)</f>
-        <v>10.581848749999999</v>
+        <v>11.5270335</v>
       </c>
       <c r="G62">
         <v>11.109626</v>
@@ -16544,7 +16698,7 @@
         <v>37</v>
       </c>
       <c r="E63">
-        <v>10.474228</v>
+        <v>11.287958</v>
       </c>
       <c r="G63">
         <v>11.109626</v>
@@ -16561,7 +16715,7 @@
         <v>38</v>
       </c>
       <c r="E64">
-        <v>10.419724</v>
+        <v>11.498381</v>
       </c>
       <c r="G64">
         <v>11.109626</v>
@@ -16578,7 +16732,7 @@
         <v>39</v>
       </c>
       <c r="E65">
-        <v>10.628868000000001</v>
+        <v>11.567627999999999</v>
       </c>
       <c r="G65">
         <v>11.109626</v>
@@ -16595,11 +16749,11 @@
         <v>34</v>
       </c>
       <c r="E66">
-        <v>9.7236550000000008</v>
+        <v>11.122528000000001</v>
       </c>
       <c r="F66">
         <f>AVERAGE(E66:E69)</f>
-        <v>9.7281172500000004</v>
+        <v>11.077177250000002</v>
       </c>
       <c r="G66">
         <v>11.253282</v>
@@ -16616,7 +16770,7 @@
         <v>37</v>
       </c>
       <c r="E67">
-        <v>9.6921990000000005</v>
+        <v>11.312289</v>
       </c>
       <c r="G67">
         <v>11.253282</v>
@@ -16633,7 +16787,7 @@
         <v>38</v>
       </c>
       <c r="E68">
-        <v>9.8228039999999996</v>
+        <v>11.107376</v>
       </c>
       <c r="G68">
         <v>11.253282</v>
@@ -16650,7 +16804,7 @@
         <v>39</v>
       </c>
       <c r="E69">
-        <v>9.6738110000000006</v>
+        <v>10.766515999999999</v>
       </c>
       <c r="G69">
         <v>11.253282</v>
@@ -16667,11 +16821,11 @@
         <v>34</v>
       </c>
       <c r="E70">
-        <v>10.454656999999999</v>
+        <v>11.709467</v>
       </c>
       <c r="F70">
         <f>AVERAGE(E70:E73)</f>
-        <v>10.27927375</v>
+        <v>11.60830275</v>
       </c>
       <c r="G70">
         <v>12.297055</v>
@@ -16688,7 +16842,7 @@
         <v>37</v>
       </c>
       <c r="E71">
-        <v>10.180792</v>
+        <v>11.741716</v>
       </c>
       <c r="G71">
         <v>12.297055</v>
@@ -16705,7 +16859,7 @@
         <v>38</v>
       </c>
       <c r="E72">
-        <v>10.18181</v>
+        <v>11.189567</v>
       </c>
       <c r="G72">
         <v>12.297055</v>
@@ -16722,7 +16876,7 @@
         <v>39</v>
       </c>
       <c r="E73">
-        <v>10.299836000000001</v>
+        <v>11.792460999999999</v>
       </c>
       <c r="G73">
         <v>12.297055</v>
@@ -16739,11 +16893,11 @@
         <v>34</v>
       </c>
       <c r="E74">
-        <v>10.557674</v>
+        <v>11.007820000000001</v>
       </c>
       <c r="F74">
         <f>AVERAGE(E74:E77)</f>
-        <v>10.739731750000001</v>
+        <v>11.219330250000001</v>
       </c>
       <c r="G74">
         <v>10.117616</v>
@@ -16760,7 +16914,7 @@
         <v>37</v>
       </c>
       <c r="E75">
-        <v>10.991721999999999</v>
+        <v>11.419343</v>
       </c>
       <c r="G75">
         <v>10.117616</v>
@@ -16777,7 +16931,7 @@
         <v>38</v>
       </c>
       <c r="E76">
-        <v>10.843082000000001</v>
+        <v>11.681285000000001</v>
       </c>
       <c r="G76">
         <v>10.117616</v>
@@ -16794,7 +16948,7 @@
         <v>39</v>
       </c>
       <c r="E77">
-        <v>10.566449</v>
+        <v>10.768872999999999</v>
       </c>
       <c r="G77">
         <v>10.117616</v>
@@ -16811,11 +16965,11 @@
         <v>34</v>
       </c>
       <c r="E78">
-        <v>12.530212000000001</v>
+        <v>13.219771</v>
       </c>
       <c r="F78">
         <f>AVERAGE(E78:E81)</f>
-        <v>11.91831575</v>
+        <v>12.991008249999998</v>
       </c>
       <c r="G78">
         <v>10.937716</v>
@@ -16832,7 +16986,7 @@
         <v>37</v>
       </c>
       <c r="E79">
-        <v>11.267878</v>
+        <v>13.181647999999999</v>
       </c>
       <c r="G79">
         <v>10.937716</v>
@@ -16849,7 +17003,7 @@
         <v>38</v>
       </c>
       <c r="E80">
-        <v>11.919216</v>
+        <v>12.741687000000001</v>
       </c>
       <c r="G80">
         <v>10.937716</v>
@@ -16866,7 +17020,7 @@
         <v>39</v>
       </c>
       <c r="E81">
-        <v>11.955957</v>
+        <v>12.820926999999999</v>
       </c>
       <c r="G81">
         <v>10.937716</v>

</xml_diff>

<commit_message>
this is still up to date. can't wait to get the final results in it though
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons_rev2.xlsx
+++ b/metaboliccostcomparisons_rev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DEBF78-4DEB-43CA-9F9A-9BA95E48266A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920E7759-E38B-469B-A627-73F612F344F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="3" r:id="rId1"/>
@@ -21,19 +21,6 @@
     <sheet name="alldata_1step" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -3652,7 +3639,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Subject 02</c:v>
           </c:tx>
@@ -3747,7 +3734,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Subject 03</c:v>
           </c:tx>
@@ -3858,10 +3845,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.9407420000000002</c:v>
+                  <c:v>9.025598500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.02410725</c:v>
+                  <c:v>9.7735107499999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3906,10 +3893,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.679057500000001</c:v>
+                  <c:v>10.55297025</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9984134999999998</c:v>
+                  <c:v>10.376536250000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3954,10 +3941,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>13.6868935</c:v>
+                  <c:v>9.1393942500000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.661610250000001</c:v>
+                  <c:v>10.002458499999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4002,10 +3989,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.8646075</c:v>
+                  <c:v>10.573042249999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.5270335</c:v>
+                  <c:v>11.120386250000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4050,10 +4037,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.077177250000002</c:v>
+                  <c:v>11.10910825</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.60830275</c:v>
+                  <c:v>11.509599499999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4098,10 +4085,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.219330250000001</c:v>
+                  <c:v>11.507214250000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.991008249999998</c:v>
+                  <c:v>12.46143575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4199,8 +4186,107 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Subject 01 Altered</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28800">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="8"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="7E0021"/>
+                    </a:solidFill>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr wrap="none"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                          <a:latin typeface="Arial"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="1"/>
+                  <c:separator> </c:separator>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$J$2:$J$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>10.656892499999998</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>11.796346249999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$H$2:$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-81DC-4D36-891B-0037244EE5A3}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
                 <c:idx val="0"/>
-                <c:order val="0"/>
+                <c:order val="1"/>
                 <c:tx>
                   <c:v>Subject 01</c:v>
                 </c:tx>
@@ -4250,16 +4336,16 @@
                   <c:showBubbleSize val="1"/>
                   <c:separator>; </c:separator>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>alldata_1step!$J$2:$J$3</c15:sqref>
                         </c15:formulaRef>
@@ -4279,8 +4365,8 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>alldata_1step!$I$2:$I$3</c15:sqref>
                         </c15:formulaRef>
@@ -4299,7 +4385,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-81DC-4D36-891B-0037244EE5A3}"/>
                   </c:ext>
@@ -4309,7 +4395,7 @@
             <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="3"/>
-                <c:order val="3"/>
+                <c:order val="4"/>
                 <c:tx>
                   <c:v>Subject 04</c:v>
                 </c:tx>
@@ -4411,105 +4497,6 @@
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-81DC-4D36-891B-0037244EE5A3}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="4"/>
-                <c:tx>
-                  <c:v>Subject 01 Altered</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28800">
-                    <a:noFill/>
-                  </a:ln>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="triangle"/>
-                  <c:size val="8"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:srgbClr val="7E0021"/>
-                    </a:solidFill>
-                  </c:spPr>
-                </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr wrap="none"/>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                          <a:latin typeface="Arial"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="0"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="1"/>
-                  <c:separator> </c:separator>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>alldata_1step!$J$2:$J$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>10.656892499999998</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>11.796346249999999</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>alldata_1step!$H$2:$H$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-81DC-4D36-891B-0037244EE5A3}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -4790,64 +4777,8 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>y=x</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:alpha val="39000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="2"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>15</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:xVal>
-          <c:yVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="2"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>15</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1BDB-4C89-873C-2104705A413C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Subject 02</c:v>
           </c:tx>
@@ -4942,7 +4873,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="4"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Subject 03</c:v>
           </c:tx>
@@ -5037,7 +4968,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:order val="5"/>
           <c:tx>
             <c:v>Subject 05</c:v>
           </c:tx>
@@ -5053,10 +4984,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8.7407420000000009</c:v>
+                  <c:v>7.8255985000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8241072500000008</c:v>
+                  <c:v>8.5735107500000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5085,7 +5016,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:order val="6"/>
           <c:tx>
             <c:v>Subject 07</c:v>
           </c:tx>
@@ -5101,10 +5032,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.4790575000000015</c:v>
+                  <c:v>9.3529702500000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7984135000000006</c:v>
+                  <c:v>9.1765362500000016</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5133,7 +5064,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:order val="7"/>
           <c:tx>
             <c:v>Subject 08</c:v>
           </c:tx>
@@ -5149,10 +5080,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12.486893500000001</c:v>
+                  <c:v>7.9393942500000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4616102500000014</c:v>
+                  <c:v>8.8024585000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5181,7 +5112,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
-          <c:order val="9"/>
+          <c:order val="8"/>
           <c:tx>
             <c:v>Subject 09</c:v>
           </c:tx>
@@ -5197,10 +5128,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.664607500000001</c:v>
+                  <c:v>9.3730422499999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.327033500000001</c:v>
+                  <c:v>9.9203862500000017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5229,7 +5160,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
-          <c:order val="10"/>
+          <c:order val="9"/>
           <c:tx>
             <c:v>Subject 10</c:v>
           </c:tx>
@@ -5245,10 +5176,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.8771772500000026</c:v>
+                  <c:v>9.909108250000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.408302750000001</c:v>
+                  <c:v>10.309599499999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5277,7 +5208,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
-          <c:order val="11"/>
+          <c:order val="10"/>
           <c:tx>
             <c:v>Subject 13</c:v>
           </c:tx>
@@ -5293,10 +5224,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.019330250000001</c:v>
+                  <c:v>10.307214250000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.791008249999999</c:v>
+                  <c:v>11.26143575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5320,6 +5251,62 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-F814-441C-92B9-813191CB1F91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>y=x</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:alpha val="39000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>15</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>15</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1BDB-4C89-873C-2104705A413C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5335,6 +5322,105 @@
         <c:axId val="64009006"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Subject 01 Altered</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28800">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="8"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="7E0021"/>
+                    </a:solidFill>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr wrap="none"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                          <a:latin typeface="Arial"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="1"/>
+                  <c:separator> </c:separator>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$K$2:$K$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>9.4568924999999986</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10.59634625</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$H$2:$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-91D1-475F-B172-92ACE69A5823}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="0"/>
@@ -5388,111 +5474,6 @@
                   <c:showBubbleSize val="1"/>
                   <c:separator>; </c:separator>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>alldata_1step!$K$2:$K$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>9.4568924999999986</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>10.59634625</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>alldata_1step!$I$2:$I$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>11.061007999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>11.276054999999999</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-91D1-475F-B172-92ACE69A5823}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:v>Subject 01 Altered</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28800">
-                    <a:noFill/>
-                  </a:ln>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="triangle"/>
-                  <c:size val="8"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:srgbClr val="7E0021"/>
-                    </a:solidFill>
-                  </c:spPr>
-                </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr wrap="none"/>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                          <a:latin typeface="Arial"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="0"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="1"/>
-                  <c:separator> </c:separator>
-                  <c:showLeaderLines val="0"/>
                   <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
@@ -5525,20 +5506,26 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>alldata_1step!$H$2:$H$3</c15:sqref>
+                          <c15:sqref>alldata_1step!$I$2:$I$3</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>11.061007999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>11.276054999999999</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-91D1-475F-B172-92ACE69A5823}"/>
+                    <c16:uniqueId val="{00000000-91D1-475F-B172-92ACE69A5823}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -5546,7 +5533,7 @@
             <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="4"/>
-                <c:order val="5"/>
+                <c:order val="4"/>
                 <c:tx>
                   <c:v>Subject 04</c:v>
                 </c:tx>
@@ -6123,22 +6110,22 @@
                   <c:v>-3.7297543833232742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-11.027620346876809</c:v>
+                  <c:v>-8.723523790997751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.7359855842192555</c:v>
+                  <c:v>1.9226644476013335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.974295812914072</c:v>
+                  <c:v>-9.80480907691868</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2688380453108823</c:v>
+                  <c:v>-5.5173658182916254</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.1029021038036015</c:v>
+                  <c:v>-3.8846441125089122</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-15.02567009059635</c:v>
+                  <c:v>-8.4733556287438674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6794,22 +6781,22 @@
                   <c:v>-6.1489278867575043</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-11.027620346876809</c:v>
+                  <c:v>-8.723523790997751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.7359855842192555</c:v>
+                  <c:v>1.9226644476013335</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.974295812914072</c:v>
+                  <c:v>-9.80480907691868</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2688380453108823</c:v>
+                  <c:v>-5.5173658182916254</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.1029021038036015</c:v>
+                  <c:v>-3.8846441125089122</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-15.02567009059635</c:v>
+                  <c:v>-8.4733556287438674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7005,122 +6992,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>alldata_1step!$N$30:$N$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>-0.21504700000000021</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.41765799999999942</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.30866300000000102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11609499999999962</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.4934899999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.16019100000000108</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.9318919999999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.2936880000000013</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.0437729999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.82010000000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-591C-44B3-A765-44177E63EE17}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ED7D31"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>alldata_1step!$O$30:$O$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>-1.1394537500000013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.75038875000000083</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.36883224999999875</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.64127275000000061</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.0833652499999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.68064400000000091</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0252832499999993</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.33757400000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.53112549999999814</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.7716779999999979</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-591C-44B3-A765-44177E63EE17}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="0"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Experimental</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="4472C4"/>
@@ -7168,40 +7044,81 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>alldata_1step!$N$30:$N$39</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$N$30:$N$39</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(alldata_1step!$N$31:$N$32,alldata_1step!$N$34:$N$39)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.21504700000000021</c:v>
+                  <c:v>-0.41765799999999942</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.41765799999999942</c:v>
+                  <c:v>-0.30866300000000102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.30866300000000102</c:v>
+                  <c:v>-1.4934899999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11609499999999962</c:v>
+                  <c:v>-0.16019100000000108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.4934899999999995</c:v>
+                  <c:v>-0.9318919999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.16019100000000108</c:v>
+                  <c:v>-1.2936880000000013</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.9318919999999995</c:v>
+                  <c:v>-1.0437729999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.2936880000000013</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.0437729999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>-0.82010000000000005</c:v>
                 </c:pt>
               </c:numCache>
@@ -7216,6 +7133,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Simulation</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="ED7D31"/>
@@ -7263,41 +7183,82 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>alldata_1step!$P$30:$P$39</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$P$30:$P$39</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(alldata_1step!$P$31:$P$32,alldata_1step!$P$34:$P$39)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-1.1394537500000013</c:v>
+                  <c:v>-0.75038875000000083</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.75038875000000083</c:v>
+                  <c:v>-0.36883224999999875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.36883224999999875</c:v>
+                  <c:v>-0.74791224999999972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.64127275000000061</c:v>
+                  <c:v>0.17643399999999865</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0833652499999999</c:v>
+                  <c:v>-0.86306424999999987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68064400000000091</c:v>
+                  <c:v>-0.5473440000000025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0252832499999993</c:v>
+                  <c:v>-0.40049124999999819</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33757400000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.53112549999999814</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.7716779999999979</c:v>
+                  <c:v>-0.95422149999999917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7320,7 +7281,218 @@
         <c:overlap val="-27"/>
         <c:axId val="38660507"/>
         <c:axId val="84186580"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="4472C4"/>
+                  </a:solidFill>
+                  <a:ln w="0">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$N$30:$N$39</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(alldata_1step!$N$31:$N$32,alldata_1step!$N$34:$N$39)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>-0.41765799999999942</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-0.30866300000000102</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-1.4934899999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-0.16019100000000108</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-0.9318919999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-1.2936880000000013</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-1.0437729999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-0.82010000000000005</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-591C-44B3-A765-44177E63EE17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="ED7D31"/>
+                  </a:solidFill>
+                  <a:ln w="0">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$R$2:$R$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(alldata_1step!$R$3:$R$4,alldata_1step!$R$6:$R$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$O$30:$O$39</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(alldata_1step!$O$31:$O$32,alldata_1step!$O$34:$O$39)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>-0.75038875000000083</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-0.36883224999999875</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-0.74791224999999883</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.17643399999999865</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-0.86306424999999898</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-0.5473440000000025</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-0.40049124999999819</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-0.95422149999999917</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-591C-44B3-A765-44177E63EE17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="38660507"/>
@@ -13910,8 +14082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BR81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14641,13 +14813,13 @@
       </c>
       <c r="N6">
         <f>(J10-J11)/J10*100</f>
-        <v>-10.898233250596382</v>
+        <v>-8.2865668132700421</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6">
         <f>(K10-K11)/K11*100</f>
-        <v>-11.027620346876809</v>
+        <v>-8.723523790997751</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -14753,13 +14925,13 @@
       </c>
       <c r="N7">
         <f>(J12-J13)/J12*100</f>
-        <v>6.3736336282485677</v>
+        <v>1.6718894853323278</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7">
         <f>(K12-K13)/K13*100</f>
-        <v>7.7359855842192555</v>
+        <v>1.9226644476013335</v>
       </c>
       <c r="R7">
         <v>7</v>
@@ -14899,13 +15071,13 @@
       </c>
       <c r="N8">
         <f>(J14-J15)/J14*100</f>
-        <v>22.103505444825732</v>
+        <v>-9.4433419370216907</v>
       </c>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8">
         <f>(K14-K15)/K15*100</f>
-        <v>31.974295812914072</v>
+        <v>-9.80480907691868</v>
       </c>
       <c r="R8">
         <v>8</v>
@@ -15033,13 +15205,13 @@
       </c>
       <c r="N9">
         <f>(J16-J17)/J16*100</f>
-        <v>2.8452184364295241</v>
+        <v>-5.1767881661496489</v>
       </c>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9">
         <f>(K16-K17)/K17*100</f>
-        <v>3.2688380453108823</v>
+        <v>-5.5173658182916254</v>
       </c>
       <c r="R9">
         <v>9</v>
@@ -15159,11 +15331,11 @@
       </c>
       <c r="J10">
         <f>F34</f>
-        <v>9.9407420000000002</v>
+        <v>9.025598500000001</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>8.7407420000000009</v>
+        <v>7.8255985000000008</v>
       </c>
       <c r="L10">
         <v>5</v>
@@ -15174,13 +15346,13 @@
       </c>
       <c r="N10">
         <f>(J18-J19)/J18*100</f>
-        <v>-4.7947729643849302</v>
+        <v>-3.6050710911021882</v>
       </c>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10">
         <f>(K18-K19)/K19*100</f>
-        <v>-5.1029021038036015</v>
+        <v>-3.8846441125089122</v>
       </c>
       <c r="R10">
         <v>10</v>
@@ -15268,11 +15440,11 @@
       </c>
       <c r="J11">
         <f>F38</f>
-        <v>11.02410725</v>
+        <v>9.7735107499999998</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>9.8241072500000008</v>
+        <v>8.5735107500000005</v>
       </c>
       <c r="L11">
         <v>5</v>
@@ -15283,13 +15455,13 @@
       </c>
       <c r="N11">
         <f>(J20-J21)/J20*100</f>
-        <v>-15.791299128573186</v>
+        <v>-8.2923762369332721</v>
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11">
         <f>(K20-K21)/K21*100</f>
-        <v>-15.02567009059635</v>
+        <v>-8.4733556287438674</v>
       </c>
       <c r="R11">
         <v>13</v>
@@ -15317,11 +15489,11 @@
       </c>
       <c r="J12">
         <f>F42</f>
-        <v>10.679057500000001</v>
+        <v>10.55297025</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>9.4790575000000015</v>
+        <v>9.3529702500000003</v>
       </c>
       <c r="L12">
         <v>7</v>
@@ -15354,11 +15526,11 @@
       </c>
       <c r="J13">
         <f>F46</f>
-        <v>9.9984134999999998</v>
+        <v>10.376536250000001</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>8.7984135000000006</v>
+        <v>9.1765362500000016</v>
       </c>
       <c r="L13">
         <v>7</v>
@@ -15396,11 +15568,11 @@
       </c>
       <c r="J14">
         <f>F50</f>
-        <v>13.6868935</v>
+        <v>9.1393942500000005</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>12.486893500000001</v>
+        <v>7.9393942500000003</v>
       </c>
       <c r="L14">
         <v>8</v>
@@ -15437,11 +15609,11 @@
       </c>
       <c r="J15">
         <f>F54</f>
-        <v>10.661610250000001</v>
+        <v>10.002458499999999</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>9.4616102500000014</v>
+        <v>8.8024585000000002</v>
       </c>
       <c r="L15">
         <v>8</v>
@@ -15471,11 +15643,11 @@
       </c>
       <c r="J16">
         <f>F58</f>
-        <v>11.8646075</v>
+        <v>10.573042249999999</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>10.664607500000001</v>
+        <v>9.3730422499999992</v>
       </c>
       <c r="L16">
         <v>9</v>
@@ -15505,11 +15677,11 @@
       </c>
       <c r="J17">
         <f>F62</f>
-        <v>11.5270335</v>
+        <v>11.120386250000001</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>10.327033500000001</v>
+        <v>9.9203862500000017</v>
       </c>
       <c r="L17">
         <v>9</v>
@@ -15543,11 +15715,11 @@
       </c>
       <c r="J18">
         <f>F66</f>
-        <v>11.077177250000002</v>
+        <v>11.10910825</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>9.8771772500000026</v>
+        <v>9.909108250000001</v>
       </c>
       <c r="L18">
         <v>10</v>
@@ -15577,11 +15749,11 @@
       </c>
       <c r="J19">
         <f>F70</f>
-        <v>11.60830275</v>
+        <v>11.509599499999998</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>10.408302750000001</v>
+        <v>10.309599499999999</v>
       </c>
       <c r="L19">
         <v>10</v>
@@ -15611,11 +15783,11 @@
       </c>
       <c r="J20">
         <f>F74</f>
-        <v>11.219330250000001</v>
+        <v>11.507214250000001</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>10.019330250000001</v>
+        <v>10.307214250000001</v>
       </c>
       <c r="L20">
         <v>13</v>
@@ -15645,11 +15817,11 @@
       </c>
       <c r="J21">
         <f>F78</f>
-        <v>12.991008249999998</v>
+        <v>12.46143575</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>11.791008249999999</v>
+        <v>11.26143575</v>
       </c>
       <c r="L21">
         <v>13</v>
@@ -15833,7 +16005,7 @@
       </c>
       <c r="I30">
         <f>AVERAGE(J30:J49)</f>
-        <v>2.3566705198385196</v>
+        <v>1.2453932240095038</v>
       </c>
       <c r="J30">
         <f>(J2-I2)^2</f>
@@ -15841,7 +16013,7 @@
       </c>
       <c r="K30">
         <f>AVERAGE(L30:L49)</f>
-        <v>1.2951884398385187</v>
+        <v>1.2791545940095033</v>
       </c>
       <c r="L30">
         <f>(K2-I2)^2</f>
@@ -15973,11 +16145,11 @@
         <v>34</v>
       </c>
       <c r="E34">
-        <v>9.7181440000000006</v>
+        <v>8.6601879999999998</v>
       </c>
       <c r="F34">
         <f>AVERAGE(E34:E37)</f>
-        <v>9.9407420000000002</v>
+        <v>9.025598500000001</v>
       </c>
       <c r="G34">
         <v>9.4284049999999997</v>
@@ -15996,11 +16168,11 @@
       </c>
       <c r="O34">
         <f>J10-J11</f>
-        <v>-1.0833652499999999</v>
+        <v>-0.74791224999999883</v>
       </c>
       <c r="P34">
         <f>K10-K11</f>
-        <v>-1.0833652499999999</v>
+        <v>-0.74791224999999972</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
@@ -16014,7 +16186,7 @@
         <v>37</v>
       </c>
       <c r="E35">
-        <v>9.7003730000000008</v>
+        <v>9.0667150000000003</v>
       </c>
       <c r="G35">
         <v>9.4284049999999997</v>
@@ -16033,11 +16205,11 @@
       </c>
       <c r="O35">
         <f>J12-J13</f>
-        <v>0.68064400000000091</v>
+        <v>0.17643399999999865</v>
       </c>
       <c r="P35">
         <f>K12-K13</f>
-        <v>0.68064400000000091</v>
+        <v>0.17643399999999865</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
@@ -16051,7 +16223,7 @@
         <v>38</v>
       </c>
       <c r="E36">
-        <v>10.118931</v>
+        <v>9.2164610000000007</v>
       </c>
       <c r="G36">
         <v>9.4284049999999997</v>
@@ -16070,11 +16242,11 @@
       </c>
       <c r="O36">
         <f>J14-J15</f>
-        <v>3.0252832499999993</v>
+        <v>-0.86306424999999898</v>
       </c>
       <c r="P36">
         <f>K14-K15</f>
-        <v>3.0252832499999993</v>
+        <v>-0.86306424999999987</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
@@ -16088,7 +16260,7 @@
         <v>39</v>
       </c>
       <c r="E37">
-        <v>10.225519999999999</v>
+        <v>9.1590299999999996</v>
       </c>
       <c r="G37">
         <v>9.4284049999999997</v>
@@ -16107,11 +16279,11 @@
       </c>
       <c r="O37">
         <f>J16-J17</f>
-        <v>0.33757400000000004</v>
+        <v>-0.5473440000000025</v>
       </c>
       <c r="P37">
         <f>K16-K17</f>
-        <v>0.33757400000000004</v>
+        <v>-0.5473440000000025</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -16125,22 +16297,22 @@
         <v>34</v>
       </c>
       <c r="E38">
-        <v>11.057202</v>
+        <v>9.9775500000000008</v>
       </c>
       <c r="F38">
         <f>AVERAGE(E38:E41)</f>
-        <v>11.02410725</v>
+        <v>9.7735107499999998</v>
       </c>
       <c r="G38">
         <v>10.921894999999999</v>
       </c>
       <c r="J38">
         <f t="shared" si="1"/>
-        <v>0.26248920156900052</v>
+        <v>0.16225307644224898</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
-        <v>0.47288040156899835</v>
+        <v>2.5689886764422467</v>
       </c>
       <c r="N38" s="14">
         <f>I18-I19</f>
@@ -16148,11 +16320,11 @@
       </c>
       <c r="O38">
         <f>J18-J19</f>
-        <v>-0.53112549999999814</v>
+        <v>-0.40049124999999819</v>
       </c>
       <c r="P38">
         <f>K18-K19</f>
-        <v>-0.53112549999999814</v>
+        <v>-0.40049124999999819</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
@@ -16166,18 +16338,18 @@
         <v>37</v>
       </c>
       <c r="E39">
-        <v>10.943826</v>
+        <v>9.4892839999999996</v>
       </c>
       <c r="G39">
         <v>10.921894999999999</v>
       </c>
       <c r="J39">
         <f t="shared" si="1"/>
-        <v>1.0447344050062682E-2</v>
+        <v>1.3187863856480613</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
-        <v>1.2051379440500589</v>
+        <v>5.5149085856480564</v>
       </c>
       <c r="N39" s="14">
         <f>I20-I21</f>
@@ -16185,11 +16357,11 @@
       </c>
       <c r="O39">
         <f>J20-J21</f>
-        <v>-1.7716779999999979</v>
+        <v>-0.95422149999999917</v>
       </c>
       <c r="P39">
         <f>K20-K21</f>
-        <v>-1.7716779999999979</v>
+        <v>-0.95422149999999917</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
@@ -16203,18 +16375,18 @@
         <v>38</v>
       </c>
       <c r="E40">
-        <v>10.924265</v>
+        <v>9.8151960000000003</v>
       </c>
       <c r="G40">
         <v>10.921894999999999</v>
       </c>
       <c r="J40">
         <f t="shared" si="1"/>
-        <v>1.6828873993822531</v>
+        <v>1.3716491238630624</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
-        <v>9.4597993822503664E-3</v>
+        <v>8.309238630624606E-4</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
@@ -16228,18 +16400,18 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <v>11.171136000000001</v>
+        <v>9.8120130000000003</v>
       </c>
       <c r="G41">
         <v>10.921894999999999</v>
       </c>
       <c r="J41">
         <f t="shared" si="1"/>
-        <v>0.20832514990224926</v>
+        <v>0.69647245067556296</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
-        <v>0.55290154990225016</v>
+        <v>0.13355425067556181</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -16253,22 +16425,22 @@
         <v>34</v>
       </c>
       <c r="E42">
-        <v>10.75526</v>
+        <v>10.547658999999999</v>
       </c>
       <c r="F42">
         <f>AVERAGE(E42:E45)</f>
-        <v>10.679057500000001</v>
+        <v>10.55297025</v>
       </c>
       <c r="G42">
         <v>9.3817959999999996</v>
       </c>
       <c r="J42">
         <f>(J14-I14)^2</f>
-        <v>18.759211147290248</v>
+        <v>4.678947532656233E-2</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
-        <v>9.8043539472902541</v>
+        <v>2.0059304753265619</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
@@ -16282,18 +16454,18 @@
         <v>37</v>
       </c>
       <c r="E43">
-        <v>10.262174</v>
+        <v>11.321642000000001</v>
       </c>
       <c r="G43">
         <v>9.3817959999999996</v>
       </c>
       <c r="J43">
         <f>(J15-I15)^2</f>
-        <v>0.13988740723256335</v>
+        <v>8.1302823632250068E-2</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
-        <v>0.68225080723255949</v>
+        <v>2.2056304236322481</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
@@ -16307,18 +16479,18 @@
         <v>38</v>
       </c>
       <c r="E44">
-        <v>10.728984000000001</v>
+        <v>10.564242999999999</v>
       </c>
       <c r="G44">
         <v>9.3817959999999996</v>
       </c>
       <c r="J44">
         <f t="shared" ref="J44:J49" si="3">(J16-I16)^2</f>
-        <v>4.1970467202302535</v>
+        <v>0.57320684536806155</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
-        <v>0.72023992023025263</v>
+        <v>0.19615664536806243</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -16332,18 +16504,18 @@
         <v>39</v>
       </c>
       <c r="E45">
-        <v>10.969811999999999</v>
+        <v>9.7783370000000005</v>
       </c>
       <c r="G45">
         <v>9.3817959999999996</v>
       </c>
       <c r="J45">
         <f t="shared" si="3"/>
-        <v>0.17422902105624957</v>
+        <v>1.1578298006251252E-4</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
-        <v>0.61245102105624971</v>
+        <v>1.4142911829800595</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -16357,22 +16529,22 @@
         <v>34</v>
       </c>
       <c r="E46">
-        <v>9.8622639999999997</v>
+        <v>11.832392</v>
       </c>
       <c r="F46">
         <f>AVERAGE(E46:E49)</f>
-        <v>9.9984134999999998</v>
+        <v>10.376536250000001</v>
       </c>
       <c r="G46">
         <v>9.5419870000000007</v>
       </c>
       <c r="J46">
         <f t="shared" si="3"/>
-        <v>3.1012882972562002E-2</v>
+        <v>2.0786070189062561E-2</v>
       </c>
       <c r="L46">
         <f t="shared" si="2"/>
-        <v>1.8936642829725567</v>
+        <v>1.8068030701890612</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
@@ -16386,18 +16558,18 @@
         <v>37</v>
       </c>
       <c r="E47">
-        <v>10.020934</v>
+        <v>10.246069</v>
       </c>
       <c r="G47">
         <v>9.5419870000000007</v>
       </c>
       <c r="J47">
         <f t="shared" si="3"/>
-        <v>0.47437966188006292</v>
+        <v>0.62008616448025289</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
-        <v>3.5673850618800609</v>
+        <v>3.9499793644802548</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
@@ -16411,18 +16583,18 @@
         <v>38</v>
       </c>
       <c r="E48">
-        <v>10.009589999999999</v>
+        <v>9.4793640000000003</v>
       </c>
       <c r="G48">
         <v>9.5419870000000007</v>
       </c>
       <c r="J48">
         <f t="shared" si="3"/>
-        <v>1.2137742886530638</v>
+        <v>1.9309832964030642</v>
       </c>
       <c r="L48">
         <f t="shared" si="2"/>
-        <v>9.6600886530622508E-3</v>
+        <v>3.5947496403062995E-2</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
@@ -16436,18 +16608,18 @@
         <v>39</v>
       </c>
       <c r="E49">
-        <v>10.100866</v>
+        <v>9.9483200000000007</v>
       </c>
       <c r="G49">
         <v>9.5419870000000007</v>
       </c>
       <c r="J49">
         <f t="shared" si="3"/>
-        <v>4.2160090639100556</v>
+        <v>2.3217218765400616</v>
       </c>
       <c r="L49">
         <f t="shared" si="2"/>
-        <v>0.72810766391006099</v>
+        <v>0.10479447654006277</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
@@ -16461,11 +16633,11 @@
         <v>34</v>
       </c>
       <c r="E50">
-        <v>9.1451019999999996</v>
+        <v>8.7803909999999998</v>
       </c>
       <c r="F50">
         <f>AVERAGE(E50:E53)</f>
-        <v>13.6868935</v>
+        <v>9.1393942500000005</v>
       </c>
       <c r="G50">
         <v>9.3557030000000001</v>
@@ -16482,7 +16654,7 @@
         <v>37</v>
       </c>
       <c r="E51">
-        <v>9.7850619999999999</v>
+        <v>9.1737330000000004</v>
       </c>
       <c r="G51">
         <v>9.3557030000000001</v>
@@ -16499,7 +16671,7 @@
         <v>38</v>
       </c>
       <c r="E52">
-        <v>18.428795000000001</v>
+        <v>9.2776730000000001</v>
       </c>
       <c r="G52">
         <v>9.3557030000000001</v>
@@ -16516,7 +16688,7 @@
         <v>39</v>
       </c>
       <c r="E53">
-        <v>17.388615000000001</v>
+        <v>9.32578</v>
       </c>
       <c r="G53">
         <v>9.3557030000000001</v>
@@ -16533,11 +16705,11 @@
         <v>34</v>
       </c>
       <c r="E54">
-        <v>10.745618</v>
+        <v>10.041607000000001</v>
       </c>
       <c r="F54">
         <f>AVERAGE(E54:E57)</f>
-        <v>10.661610250000001</v>
+        <v>10.002458499999999</v>
       </c>
       <c r="G54">
         <v>10.287595</v>
@@ -16554,7 +16726,7 @@
         <v>37</v>
       </c>
       <c r="E55">
-        <v>10.12487</v>
+        <v>9.8198120000000007</v>
       </c>
       <c r="G55">
         <v>10.287595</v>
@@ -16571,7 +16743,7 @@
         <v>38</v>
       </c>
       <c r="E56">
-        <v>11.157829</v>
+        <v>10.293556000000001</v>
       </c>
       <c r="G56">
         <v>10.287595</v>
@@ -16588,7 +16760,7 @@
         <v>39</v>
       </c>
       <c r="E57">
-        <v>10.618124</v>
+        <v>9.8548589999999994</v>
       </c>
       <c r="G57">
         <v>10.287595</v>
@@ -16605,11 +16777,11 @@
         <v>34</v>
       </c>
       <c r="E58">
-        <v>10.987154</v>
+        <v>10.363528000000001</v>
       </c>
       <c r="F58">
         <f>AVERAGE(E58:E61)</f>
-        <v>11.8646075</v>
+        <v>10.573042249999999</v>
       </c>
       <c r="G58">
         <v>9.8159379999999992</v>
@@ -16626,7 +16798,7 @@
         <v>37</v>
       </c>
       <c r="E59">
-        <v>14.224887000000001</v>
+        <v>9.9679210000000005</v>
       </c>
       <c r="G59">
         <v>9.8159379999999992</v>
@@ -16643,7 +16815,7 @@
         <v>38</v>
       </c>
       <c r="E60">
-        <v>11.454666</v>
+        <v>11.168996999999999</v>
       </c>
       <c r="G60">
         <v>9.8159379999999992</v>
@@ -16677,11 +16849,11 @@
         <v>34</v>
       </c>
       <c r="E62">
-        <v>11.754167000000001</v>
+        <v>11.357813</v>
       </c>
       <c r="F62">
         <f>AVERAGE(E62:E65)</f>
-        <v>11.5270335</v>
+        <v>11.120386250000001</v>
       </c>
       <c r="G62">
         <v>11.109626</v>
@@ -16698,7 +16870,7 @@
         <v>37</v>
       </c>
       <c r="E63">
-        <v>11.287958</v>
+        <v>10.975279</v>
       </c>
       <c r="G63">
         <v>11.109626</v>
@@ -16715,7 +16887,7 @@
         <v>38</v>
       </c>
       <c r="E64">
-        <v>11.498381</v>
+        <v>11.072824000000001</v>
       </c>
       <c r="G64">
         <v>11.109626</v>
@@ -16732,7 +16904,7 @@
         <v>39</v>
       </c>
       <c r="E65">
-        <v>11.567627999999999</v>
+        <v>11.075628999999999</v>
       </c>
       <c r="G65">
         <v>11.109626</v>
@@ -16749,11 +16921,11 @@
         <v>34</v>
       </c>
       <c r="E66">
-        <v>11.122528000000001</v>
+        <v>11.109363</v>
       </c>
       <c r="F66">
         <f>AVERAGE(E66:E69)</f>
-        <v>11.077177250000002</v>
+        <v>11.10910825</v>
       </c>
       <c r="G66">
         <v>11.253282</v>
@@ -16770,7 +16942,7 @@
         <v>37</v>
       </c>
       <c r="E67">
-        <v>11.312289</v>
+        <v>11.107533</v>
       </c>
       <c r="G67">
         <v>11.253282</v>
@@ -16787,7 +16959,7 @@
         <v>38</v>
       </c>
       <c r="E68">
-        <v>11.107376</v>
+        <v>11.141007</v>
       </c>
       <c r="G68">
         <v>11.253282</v>
@@ -16804,7 +16976,7 @@
         <v>39</v>
       </c>
       <c r="E69">
-        <v>10.766515999999999</v>
+        <v>11.078530000000001</v>
       </c>
       <c r="G69">
         <v>11.253282</v>
@@ -16821,11 +16993,11 @@
         <v>34</v>
       </c>
       <c r="E70">
-        <v>11.709467</v>
+        <v>11.145773999999999</v>
       </c>
       <c r="F70">
         <f>AVERAGE(E70:E73)</f>
-        <v>11.60830275</v>
+        <v>11.509599499999998</v>
       </c>
       <c r="G70">
         <v>12.297055</v>
@@ -16842,7 +17014,7 @@
         <v>37</v>
       </c>
       <c r="E71">
-        <v>11.741716</v>
+        <v>11.527557</v>
       </c>
       <c r="G71">
         <v>12.297055</v>
@@ -16859,7 +17031,7 @@
         <v>38</v>
       </c>
       <c r="E72">
-        <v>11.189567</v>
+        <v>11.008775999999999</v>
       </c>
       <c r="G72">
         <v>12.297055</v>
@@ -16876,7 +17048,7 @@
         <v>39</v>
       </c>
       <c r="E73">
-        <v>11.792460999999999</v>
+        <v>12.356291000000001</v>
       </c>
       <c r="G73">
         <v>12.297055</v>
@@ -16893,11 +17065,11 @@
         <v>34</v>
       </c>
       <c r="E74">
-        <v>11.007820000000001</v>
+        <v>11.589969</v>
       </c>
       <c r="F74">
         <f>AVERAGE(E74:E77)</f>
-        <v>11.219330250000001</v>
+        <v>11.507214250000001</v>
       </c>
       <c r="G74">
         <v>10.117616</v>
@@ -16914,7 +17086,7 @@
         <v>37</v>
       </c>
       <c r="E75">
-        <v>11.419343</v>
+        <v>11.70552</v>
       </c>
       <c r="G75">
         <v>10.117616</v>
@@ -16931,7 +17103,7 @@
         <v>38</v>
       </c>
       <c r="E76">
-        <v>11.681285000000001</v>
+        <v>11.39451</v>
       </c>
       <c r="G76">
         <v>10.117616</v>
@@ -16948,7 +17120,7 @@
         <v>39</v>
       </c>
       <c r="E77">
-        <v>10.768872999999999</v>
+        <v>11.338858</v>
       </c>
       <c r="G77">
         <v>10.117616</v>
@@ -16965,11 +17137,11 @@
         <v>34</v>
       </c>
       <c r="E78">
-        <v>13.219771</v>
+        <v>12.432638000000001</v>
       </c>
       <c r="F78">
         <f>AVERAGE(E78:E81)</f>
-        <v>12.991008249999998</v>
+        <v>12.46143575</v>
       </c>
       <c r="G78">
         <v>10.937716</v>
@@ -16986,7 +17158,7 @@
         <v>37</v>
       </c>
       <c r="E79">
-        <v>13.181647999999999</v>
+        <v>12.816719000000001</v>
       </c>
       <c r="G79">
         <v>10.937716</v>
@@ -17003,7 +17175,7 @@
         <v>38</v>
       </c>
       <c r="E80">
-        <v>12.741687000000001</v>
+        <v>12.255646</v>
       </c>
       <c r="G80">
         <v>10.937716</v>
@@ -17020,7 +17192,7 @@
         <v>39</v>
       </c>
       <c r="E81">
-        <v>12.820926999999999</v>
+        <v>12.34074</v>
       </c>
       <c r="G81">
         <v>10.937716</v>

</xml_diff>

<commit_message>
General updates. The excel files are not the final results, but some random step in the process.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons_rev2.xlsx
+++ b/metaboliccostcomparisons_rev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920E7759-E38B-469B-A627-73F612F344F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB9BB4C-8C59-48F6-9656-1E1799051FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2010" yWindow="1980" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="3" r:id="rId1"/>
@@ -21,11 +21,24 @@
     <sheet name="alldata_1step" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="131">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -369,9 +382,6 @@
     <t>percent reduction simulation without basal</t>
   </si>
   <si>
-    <t>Squared error</t>
-  </si>
-  <si>
     <t>Squared error without basal</t>
   </si>
   <si>
@@ -379,6 +389,48 @@
   </si>
   <si>
     <t>subject</t>
+  </si>
+  <si>
+    <t>RMS error without basal</t>
+  </si>
+  <si>
+    <t>peak RMS</t>
+  </si>
+  <si>
+    <t>peak error</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>average natural experiment</t>
+  </si>
+  <si>
+    <t>average exo experiment</t>
+  </si>
+  <si>
+    <t>average natural simulation w/o basal</t>
+  </si>
+  <si>
+    <t>average exo simulation w/o basal</t>
+  </si>
+  <si>
+    <t>average experiment difference</t>
+  </si>
+  <si>
+    <t>average simulation difference</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max 3%</t>
+  </si>
+  <si>
+    <t>min 3%</t>
   </si>
 </sst>
 </file>
@@ -388,7 +440,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -414,6 +466,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -537,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -557,6 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3845,10 +3904,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.025598500000001</c:v>
+                  <c:v>9.8343617500000011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7735107499999998</c:v>
+                  <c:v>12.667466749999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3893,10 +3952,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.55297025</c:v>
+                  <c:v>11.302342999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.376536250000001</c:v>
+                  <c:v>10.78000525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3941,10 +4000,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.1393942500000005</c:v>
+                  <c:v>9.144444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.002458499999999</c:v>
+                  <c:v>9.9639717499999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3989,10 +4048,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.573042249999999</c:v>
+                  <c:v>10.167945</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.120386250000001</c:v>
+                  <c:v>11.200957750000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4037,10 +4096,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.10910825</c:v>
+                  <c:v>10.61172225</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.509599499999998</c:v>
+                  <c:v>10.983643999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4085,10 +4144,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.507214250000001</c:v>
+                  <c:v>10.394560500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.46143575</c:v>
+                  <c:v>12.34157525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4272,6 +4331,12 @@
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
@@ -4984,10 +5049,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.8255985000000008</c:v>
+                  <c:v>8.6343617500000018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5735107500000005</c:v>
+                  <c:v>11.46746675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5032,10 +5097,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.3529702500000003</c:v>
+                  <c:v>10.102342999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1765362500000016</c:v>
+                  <c:v>9.580005250000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5080,10 +5145,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.9393942500000003</c:v>
+                  <c:v>7.9444439999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8024585000000002</c:v>
+                  <c:v>8.7639717499999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5128,10 +5193,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.3730422499999992</c:v>
+                  <c:v>8.9679450000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9203862500000017</c:v>
+                  <c:v>10.000957750000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5176,10 +5241,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.909108250000001</c:v>
+                  <c:v>9.4117222500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.309599499999999</c:v>
+                  <c:v>9.7836439999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5224,10 +5289,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10.307214250000001</c:v>
+                  <c:v>9.1945605000000015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.26143575</c:v>
+                  <c:v>11.141575250000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5410,6 +5475,12 @@
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
@@ -6110,22 +6181,22 @@
                   <c:v>-3.7297543833232742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.723523790997751</c:v>
+                  <c:v>-24.705587221345098</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9226644476013335</c:v>
+                  <c:v>5.4523743606507766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-9.80480907691868</c:v>
+                  <c:v>-9.3510998594900734</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.5173658182916254</c:v>
+                  <c:v>-10.329138226786338</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.8846441125089122</c:v>
+                  <c:v>-3.8014644645696283</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-8.4733556287438674</c:v>
+                  <c:v>-17.475219673268366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6781,22 +6852,22 @@
                   <c:v>-6.1489278867575043</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.723523790997751</c:v>
+                  <c:v>-24.705587221345098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9226644476013335</c:v>
+                  <c:v>5.4523743606507766</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.80480907691868</c:v>
+                  <c:v>-9.3510998594900734</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.5173658182916254</c:v>
+                  <c:v>-10.329138226786338</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-3.8846441125089122</c:v>
+                  <c:v>-3.8014644645696283</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-8.4733556287438674</c:v>
+                  <c:v>-17.475219673268366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7243,22 +7314,22 @@
                   <c:v>-0.36883224999999875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.74791224999999972</c:v>
+                  <c:v>-2.833104999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17643399999999865</c:v>
+                  <c:v>0.52233774999999838</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.86306424999999987</c:v>
+                  <c:v>-0.81952774999999978</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.5473440000000025</c:v>
+                  <c:v>-1.033012750000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.40049124999999819</c:v>
+                  <c:v>-0.3719217499999985</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.95422149999999917</c:v>
+                  <c:v>-1.9470147499999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7464,27 +7535,27 @@
                         <c:v>-0.36883224999999875</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>-0.74791224999999883</c:v>
+                        <c:v>-2.833104999999998</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.17643399999999865</c:v>
+                        <c:v>0.52233774999999838</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>-0.86306424999999898</c:v>
+                        <c:v>-0.81952774999999889</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>-0.5473440000000025</c:v>
+                        <c:v>-1.033012750000001</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>-0.40049124999999819</c:v>
+                        <c:v>-0.3719217499999985</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>-0.95422149999999917</c:v>
+                        <c:v>-1.9470147499999992</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-591C-44B3-A765-44177E63EE17}"/>
                   </c:ext>
@@ -8408,13 +8479,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>846825</xdr:colOff>
+      <xdr:colOff>891649</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>80257</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1698281</xdr:colOff>
+      <xdr:colOff>913869</xdr:colOff>
       <xdr:row>92</xdr:row>
       <xdr:rowOff>487</xdr:rowOff>
     </xdr:to>
@@ -8444,13 +8515,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1058751</xdr:colOff>
+      <xdr:colOff>1047545</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>108136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>330166</xdr:colOff>
+      <xdr:colOff>318960</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>51075</xdr:rowOff>
     </xdr:to>
@@ -8522,7 +8593,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>179412</xdr:colOff>
+      <xdr:colOff>179411</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>12006</xdr:rowOff>
     </xdr:to>
@@ -8558,7 +8629,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
-      <xdr:colOff>556723</xdr:colOff>
+      <xdr:colOff>556722</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>5801</xdr:rowOff>
     </xdr:to>
@@ -8594,7 +8665,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>70</xdr:col>
-      <xdr:colOff>311620</xdr:colOff>
+      <xdr:colOff>311617</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>5801</xdr:rowOff>
     </xdr:to>
@@ -14080,10 +14151,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:BR81"/>
+  <dimension ref="A1:BR149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14092,14 +14163,14 @@
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.140625" customWidth="1"/>
     <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.7109375" bestFit="1" customWidth="1"/>
@@ -14143,6 +14214,9 @@
       <c r="G1" t="s">
         <v>19</v>
       </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
       <c r="I1" t="s">
         <v>46</v>
       </c>
@@ -14171,7 +14245,7 @@
         <v>113</v>
       </c>
       <c r="R1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AF1" t="s">
         <v>85</v>
@@ -14232,6 +14306,9 @@
       <c r="G2">
         <v>11.061007999999999</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
       <c r="I2">
         <f>AVERAGE(G2:G5)</f>
         <v>11.061007999999999</v>
@@ -14335,6 +14412,9 @@
       <c r="G3">
         <v>11.061007999999999</v>
       </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
       <c r="I3">
         <f>AVERAGE(G6:G9)</f>
         <v>11.276054999999999</v>
@@ -14495,6 +14575,9 @@
       <c r="G4">
         <v>11.061007999999999</v>
       </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
       <c r="I4">
         <f>AVERAGE(G10:G13)</f>
         <v>8.9729109999999999</v>
@@ -14641,6 +14724,9 @@
       <c r="G5">
         <v>11.061007999999999</v>
       </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
       <c r="I5">
         <f>AVERAGE(G14:G17)</f>
         <v>9.3905689999999993</v>
@@ -14792,6 +14878,9 @@
       <c r="G6">
         <v>11.276054999999999</v>
       </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
       <c r="I6">
         <f>AVERAGE(G18:G21)</f>
         <v>9.5206529999999994</v>
@@ -14813,13 +14902,13 @@
       </c>
       <c r="N6">
         <f>(J10-J11)/J10*100</f>
-        <v>-8.2865668132700421</v>
+        <v>-28.808224387312148</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6">
         <f>(K10-K11)/K11*100</f>
-        <v>-8.723523790997751</v>
+        <v>-24.705587221345098</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -14904,6 +14993,9 @@
       <c r="G7">
         <v>11.276054999999999</v>
       </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
       <c r="I7">
         <f>AVERAGE(G22:G25)</f>
         <v>9.8293160000000004</v>
@@ -14925,13 +15017,13 @@
       </c>
       <c r="N7">
         <f>(J12-J13)/J12*100</f>
-        <v>1.6718894853323278</v>
+        <v>4.6214997191290204</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7">
         <f>(K12-K13)/K13*100</f>
-        <v>1.9226644476013335</v>
+        <v>5.4523743606507766</v>
       </c>
       <c r="R7">
         <v>7</v>
@@ -15050,6 +15142,9 @@
       <c r="G8">
         <v>11.276054999999999</v>
       </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
       <c r="I8">
         <f>AVERAGE(G26:G29)</f>
         <v>9.1254899999999992</v>
@@ -15071,13 +15166,13 @@
       </c>
       <c r="N8">
         <f>(J14-J15)/J14*100</f>
-        <v>-9.4433419370216907</v>
+        <v>-8.9620292934157497</v>
       </c>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8">
         <f>(K14-K15)/K15*100</f>
-        <v>-9.80480907691868</v>
+        <v>-9.3510998594900734</v>
       </c>
       <c r="R8">
         <v>8</v>
@@ -15184,6 +15279,9 @@
       <c r="G9">
         <v>11.276054999999999</v>
       </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
       <c r="I9">
         <f>AVERAGE(G30:G33)</f>
         <v>9.0093949999999996</v>
@@ -15205,13 +15303,13 @@
       </c>
       <c r="N9">
         <f>(J16-J17)/J16*100</f>
-        <v>-5.1767881661496489</v>
+        <v>-10.159503714860781</v>
       </c>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9">
         <f>(K16-K17)/K17*100</f>
-        <v>-5.5173658182916254</v>
+        <v>-10.329138226786338</v>
       </c>
       <c r="R9">
         <v>9</v>
@@ -15325,17 +15423,20 @@
       <c r="G10">
         <v>8.9729109999999999</v>
       </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
       <c r="I10">
         <f>AVERAGE(G34:G37)</f>
         <v>9.4284049999999997</v>
       </c>
       <c r="J10">
         <f>F34</f>
-        <v>9.025598500000001</v>
+        <v>9.8343617500000011</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>7.8255985000000008</v>
+        <v>8.6343617500000018</v>
       </c>
       <c r="L10">
         <v>5</v>
@@ -15346,13 +15447,13 @@
       </c>
       <c r="N10">
         <f>(J18-J19)/J18*100</f>
-        <v>-3.6050710911021882</v>
+        <v>-3.5048198703089737</v>
       </c>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10">
         <f>(K18-K19)/K19*100</f>
-        <v>-3.8846441125089122</v>
+        <v>-3.8014644645696283</v>
       </c>
       <c r="R10">
         <v>10</v>
@@ -15434,17 +15535,20 @@
       <c r="G11">
         <v>8.9729109999999999</v>
       </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
       <c r="I11">
         <f>AVERAGE(G38:G41)</f>
         <v>10.921894999999999</v>
       </c>
       <c r="J11">
         <f>F38</f>
-        <v>9.7735107499999998</v>
+        <v>12.667466749999999</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>8.5735107500000005</v>
+        <v>11.46746675</v>
       </c>
       <c r="L11">
         <v>5</v>
@@ -15455,13 +15559,13 @@
       </c>
       <c r="N11">
         <f>(J20-J21)/J20*100</f>
-        <v>-8.2923762369332721</v>
+        <v>-18.73109257481352</v>
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11">
         <f>(K20-K21)/K21*100</f>
-        <v>-8.4733556287438674</v>
+        <v>-17.475219673268366</v>
       </c>
       <c r="R11">
         <v>13</v>
@@ -15483,17 +15587,20 @@
       <c r="G12">
         <v>8.9729109999999999</v>
       </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
       <c r="I12">
         <f>AVERAGE(G42:G45)</f>
         <v>9.3817959999999996</v>
       </c>
       <c r="J12">
         <f>F42</f>
-        <v>10.55297025</v>
+        <v>11.302342999999999</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>9.3529702500000003</v>
+        <v>10.102342999999999</v>
       </c>
       <c r="L12">
         <v>7</v>
@@ -15520,17 +15627,20 @@
       <c r="G13">
         <v>8.9729109999999999</v>
       </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
       <c r="I13">
         <f>AVERAGE(G46:G49)</f>
         <v>9.5419870000000007</v>
       </c>
       <c r="J13">
         <f>F46</f>
-        <v>10.376536250000001</v>
+        <v>10.78000525</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>9.1765362500000016</v>
+        <v>9.580005250000001</v>
       </c>
       <c r="L13">
         <v>7</v>
@@ -15562,17 +15672,20 @@
       <c r="G14">
         <v>9.3905689999999993</v>
       </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
       <c r="I14">
         <f>AVERAGE(G50:G53)</f>
         <v>9.3557030000000001</v>
       </c>
       <c r="J14">
         <f>F50</f>
-        <v>9.1393942500000005</v>
+        <v>9.144444</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>7.9393942500000003</v>
+        <v>7.9444439999999998</v>
       </c>
       <c r="L14">
         <v>8</v>
@@ -15603,17 +15716,20 @@
       <c r="G15">
         <v>9.3905689999999993</v>
       </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
       <c r="I15">
         <f>AVERAGE(G54:G57)</f>
         <v>10.287595</v>
       </c>
       <c r="J15">
         <f>F54</f>
-        <v>10.002458499999999</v>
+        <v>9.9639717499999989</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>8.8024585000000002</v>
+        <v>8.7639717499999996</v>
       </c>
       <c r="L15">
         <v>8</v>
@@ -15637,17 +15753,20 @@
       <c r="G16">
         <v>9.3905689999999993</v>
       </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
       <c r="I16">
         <f>AVERAGE(G58:G61)</f>
         <v>9.8159379999999992</v>
       </c>
       <c r="J16">
         <f>F58</f>
-        <v>10.573042249999999</v>
+        <v>10.167945</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>9.3730422499999992</v>
+        <v>8.9679450000000003</v>
       </c>
       <c r="L16">
         <v>9</v>
@@ -15671,17 +15790,20 @@
       <c r="G17">
         <v>9.3905689999999993</v>
       </c>
+      <c r="H17">
+        <v>9</v>
+      </c>
       <c r="I17">
         <f>AVERAGE(G62:G65)</f>
         <v>11.109626</v>
       </c>
       <c r="J17">
         <f>F62</f>
-        <v>11.120386250000001</v>
+        <v>11.200957750000001</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>9.9203862500000017</v>
+        <v>10.000957750000001</v>
       </c>
       <c r="L17">
         <v>9</v>
@@ -15709,17 +15831,20 @@
       <c r="G18">
         <v>9.5206529999999994</v>
       </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
       <c r="I18">
         <f>AVERAGE(G66:G69)</f>
         <v>11.253282</v>
       </c>
       <c r="J18">
         <f>F66</f>
-        <v>11.10910825</v>
+        <v>10.61172225</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>9.909108250000001</v>
+        <v>9.4117222500000004</v>
       </c>
       <c r="L18">
         <v>10</v>
@@ -15743,17 +15868,20 @@
       <c r="G19">
         <v>9.5206529999999994</v>
       </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
       <c r="I19">
         <f>AVERAGE(G70:G73)</f>
         <v>12.297055</v>
       </c>
       <c r="J19">
         <f>F70</f>
-        <v>11.509599499999998</v>
+        <v>10.983643999999998</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>10.309599499999999</v>
+        <v>9.7836439999999989</v>
       </c>
       <c r="L19">
         <v>10</v>
@@ -15777,17 +15905,20 @@
       <c r="G20">
         <v>9.5206529999999994</v>
       </c>
+      <c r="H20">
+        <v>13</v>
+      </c>
       <c r="I20">
         <f>AVERAGE(G74:G77)</f>
         <v>10.117616</v>
       </c>
       <c r="J20">
         <f>F74</f>
-        <v>11.507214250000001</v>
+        <v>10.394560500000001</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>10.307214250000001</v>
+        <v>9.1945605000000015</v>
       </c>
       <c r="L20">
         <v>13</v>
@@ -15811,17 +15942,20 @@
       <c r="G21">
         <v>9.5206529999999994</v>
       </c>
+      <c r="H21">
+        <v>13</v>
+      </c>
       <c r="I21">
         <f>AVERAGE(G78:G81)</f>
         <v>10.937716</v>
       </c>
       <c r="J21">
         <f>F78</f>
-        <v>12.46143575</v>
+        <v>12.34157525</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>11.26143575</v>
+        <v>11.141575250000001</v>
       </c>
       <c r="L21">
         <v>13</v>
@@ -15868,6 +16002,12 @@
       <c r="G23">
         <v>9.8293160000000004</v>
       </c>
+      <c r="I23" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" t="s">
+        <v>129</v>
+      </c>
       <c r="O23" s="13" t="s">
         <v>42</v>
       </c>
@@ -15889,6 +16029,14 @@
       <c r="G24">
         <v>9.8293160000000004</v>
       </c>
+      <c r="I24">
+        <f>MAX(I4:I7,I10:I21)</f>
+        <v>12.297055</v>
+      </c>
+      <c r="J24">
+        <f>0.03*I24</f>
+        <v>0.36891164999999998</v>
+      </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -15906,6 +16054,12 @@
       <c r="G25">
         <v>9.8293160000000004</v>
       </c>
+      <c r="I25" t="s">
+        <v>128</v>
+      </c>
+      <c r="J25" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -15923,6 +16077,14 @@
       <c r="G26">
         <v>9.1254899999999992</v>
       </c>
+      <c r="I26">
+        <f>MIN(I4:I7,I10:I21)</f>
+        <v>8.9729109999999999</v>
+      </c>
+      <c r="J26">
+        <f>0.03*I26</f>
+        <v>0.26918733</v>
+      </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -15965,17 +16127,20 @@
       <c r="G29">
         <v>9.1254899999999992</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="15" t="s">
         <v>53</v>
       </c>
       <c r="J29" t="s">
+        <v>120</v>
+      </c>
+      <c r="K29" t="s">
+        <v>115</v>
+      </c>
+      <c r="L29" t="s">
         <v>114</v>
       </c>
-      <c r="K29" t="s">
-        <v>116</v>
-      </c>
-      <c r="L29" t="s">
-        <v>115</v>
+      <c r="M29" t="s">
+        <v>117</v>
       </c>
       <c r="N29" t="s">
         <v>90</v>
@@ -16005,20 +16170,24 @@
       </c>
       <c r="I30">
         <f>AVERAGE(J30:J49)</f>
-        <v>1.2453932240095038</v>
+        <v>0.86692733749999995</v>
       </c>
       <c r="J30">
-        <f>(J2-I2)^2</f>
-        <v>0.16330933734025113</v>
+        <f>ABS(K2-I2)</f>
+        <v>1.6041155000000007</v>
       </c>
       <c r="K30">
         <f>AVERAGE(L30:L49)</f>
-        <v>1.2791545940095033</v>
+        <v>1.1978773649856473</v>
       </c>
       <c r="L30">
         <f>(K2-I2)^2</f>
         <v>2.573186537340252</v>
       </c>
+      <c r="M30">
+        <f>SQRT(AVERAGE(L32:L35,L38:L49))</f>
+        <v>1.0743733179766011</v>
+      </c>
       <c r="N30" s="14">
         <f>I2-I3</f>
         <v>-0.21504700000000021</v>
@@ -16046,8 +16215,8 @@
         <v>9.0093949999999996</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31:J41" si="1">(J3-I3)^2</f>
-        <v>0.27070298482656213</v>
+        <f t="shared" ref="J31:J49" si="1">ABS(K3-I3)</f>
+        <v>0.67970874999999964</v>
       </c>
       <c r="L31">
         <f t="shared" ref="L31:L49" si="2">(K3-I3)^2</f>
@@ -16079,14 +16248,20 @@
       <c r="G32">
         <v>9.0093949999999996</v>
       </c>
+      <c r="I32" t="s">
+        <v>121</v>
+      </c>
       <c r="J32">
         <f t="shared" si="1"/>
-        <v>0.6611332362009994</v>
+        <v>0.38689899999999966</v>
       </c>
       <c r="L32">
         <f t="shared" si="2"/>
         <v>0.14969083620099974</v>
       </c>
+      <c r="M32" t="s">
+        <v>119</v>
+      </c>
       <c r="N32" s="14">
         <f>I6-I7</f>
         <v>-0.30866300000000102</v>
@@ -16113,14 +16288,22 @@
       <c r="G33">
         <v>9.0093949999999996</v>
       </c>
+      <c r="I33">
+        <f>AVERAGE(I5,I7,I11,I13,I15,I17,I19,I21)</f>
+        <v>10.539469874999998</v>
+      </c>
       <c r="J33">
         <f t="shared" si="1"/>
-        <v>1.3129303993080648</v>
+        <v>5.4168249999998253E-2</v>
       </c>
       <c r="L33">
         <f t="shared" si="2"/>
         <v>2.9341993080623107E-3</v>
       </c>
+      <c r="M33">
+        <f>MAX(J32:J35,J38:J49)</f>
+        <v>2.5134110000000014</v>
+      </c>
       <c r="N33" s="14">
         <f>I8-I9</f>
         <v>0.11609499999999962</v>
@@ -16145,18 +16328,21 @@
         <v>34</v>
       </c>
       <c r="E34">
-        <v>8.6601879999999998</v>
+        <v>9.1992360000000009</v>
       </c>
       <c r="F34">
         <f>AVERAGE(E34:E37)</f>
-        <v>9.025598500000001</v>
+        <v>9.8343617500000011</v>
       </c>
       <c r="G34">
         <v>9.4284049999999997</v>
       </c>
+      <c r="I34" t="s">
+        <v>122</v>
+      </c>
       <c r="J34">
         <f t="shared" si="1"/>
-        <v>1.4386323249000033</v>
+        <v>5.6999999999796103E-4</v>
       </c>
       <c r="L34">
         <f t="shared" si="2"/>
@@ -16168,11 +16354,11 @@
       </c>
       <c r="O34">
         <f>J10-J11</f>
-        <v>-0.74791224999999883</v>
+        <v>-2.833104999999998</v>
       </c>
       <c r="P34">
         <f>K10-K11</f>
-        <v>-0.74791224999999972</v>
+        <v>-2.833104999999998</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
@@ -16186,14 +16372,18 @@
         <v>37</v>
       </c>
       <c r="E35">
-        <v>9.0667150000000003</v>
+        <v>9.1908220000000007</v>
       </c>
       <c r="G35">
         <v>9.4284049999999997</v>
       </c>
+      <c r="I35">
+        <f>AVERAGE(I20,I18,I16,I14,I12,I10,I6,I4)</f>
+        <v>9.7307879999999987</v>
+      </c>
       <c r="J35">
         <f t="shared" si="1"/>
-        <v>1.5865902706005601</v>
+        <v>5.959924999999977E-2</v>
       </c>
       <c r="L35">
         <f t="shared" si="2"/>
@@ -16205,11 +16395,11 @@
       </c>
       <c r="O35">
         <f>J12-J13</f>
-        <v>0.17643399999999865</v>
+        <v>0.52233774999999838</v>
       </c>
       <c r="P35">
         <f>K12-K13</f>
-        <v>0.17643399999999865</v>
+        <v>0.52233774999999838</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
@@ -16223,14 +16413,17 @@
         <v>38</v>
       </c>
       <c r="E36">
-        <v>9.2164610000000007</v>
+        <v>11.342254000000001</v>
       </c>
       <c r="G36">
         <v>9.4284049999999997</v>
       </c>
+      <c r="I36" t="s">
+        <v>123</v>
+      </c>
       <c r="J36">
         <f t="shared" si="1"/>
-        <v>3.4679918227702524</v>
+        <v>0.6622545000000013</v>
       </c>
       <c r="L36">
         <f t="shared" si="2"/>
@@ -16242,11 +16435,11 @@
       </c>
       <c r="O36">
         <f>J14-J15</f>
-        <v>-0.86306424999999898</v>
+        <v>-0.81952774999999889</v>
       </c>
       <c r="P36">
         <f>K14-K15</f>
-        <v>-0.86306424999999987</v>
+        <v>-0.81952774999999978</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
@@ -16260,14 +16453,18 @@
         <v>39</v>
       </c>
       <c r="E37">
-        <v>9.1590299999999996</v>
+        <v>9.6051350000000006</v>
       </c>
       <c r="G37">
         <v>9.4284049999999997</v>
       </c>
+      <c r="I37">
+        <f>AVERAGE(K5,K7,K11,K13,K15,K17,K19,K21)</f>
+        <v>9.9953670937499997</v>
+      </c>
       <c r="J37">
         <f t="shared" si="1"/>
-        <v>6.8624207326950666</v>
+        <v>1.4196222500000015</v>
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
@@ -16279,11 +16476,11 @@
       </c>
       <c r="O37">
         <f>J16-J17</f>
-        <v>-0.5473440000000025</v>
+        <v>-1.033012750000001</v>
       </c>
       <c r="P37">
         <f>K16-K17</f>
-        <v>-0.5473440000000025</v>
+        <v>-1.033012750000001</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -16297,22 +16494,25 @@
         <v>34</v>
       </c>
       <c r="E38">
-        <v>9.9775500000000008</v>
+        <v>10.902462</v>
       </c>
       <c r="F38">
         <f>AVERAGE(E38:E41)</f>
-        <v>9.7735107499999998</v>
+        <v>12.667466749999999</v>
       </c>
       <c r="G38">
         <v>10.921894999999999</v>
       </c>
+      <c r="I38" t="s">
+        <v>124</v>
+      </c>
       <c r="J38">
         <f t="shared" si="1"/>
-        <v>0.16225307644224898</v>
+        <v>0.79404324999999787</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
-        <v>2.5689886764422467</v>
+        <v>0.63050468287055916</v>
       </c>
       <c r="N38" s="14">
         <f>I18-I19</f>
@@ -16320,11 +16520,11 @@
       </c>
       <c r="O38">
         <f>J18-J19</f>
-        <v>-0.40049124999999819</v>
+        <v>-0.3719217499999985</v>
       </c>
       <c r="P38">
         <f>K18-K19</f>
-        <v>-0.40049124999999819</v>
+        <v>-0.3719217499999985</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
@@ -16338,18 +16538,22 @@
         <v>37</v>
       </c>
       <c r="E39">
-        <v>9.4892839999999996</v>
+        <v>13.13696</v>
       </c>
       <c r="G39">
         <v>10.921894999999999</v>
       </c>
+      <c r="I39">
+        <f>AVERAGE(K4,K6,K10,K12,K14,K16,K18,K20)</f>
+        <v>9.0451839374999992</v>
+      </c>
       <c r="J39">
         <f t="shared" si="1"/>
-        <v>1.3187863856480613</v>
+        <v>0.54557175000000058</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
-        <v>5.5149085856480564</v>
+        <v>0.2976485343980631</v>
       </c>
       <c r="N39" s="14">
         <f>I20-I21</f>
@@ -16357,11 +16561,11 @@
       </c>
       <c r="O39">
         <f>J20-J21</f>
-        <v>-0.95422149999999917</v>
+        <v>-1.9470147499999992</v>
       </c>
       <c r="P39">
         <f>K20-K21</f>
-        <v>-0.95422149999999917</v>
+        <v>-1.9470147499999992</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
@@ -16375,18 +16579,18 @@
         <v>38</v>
       </c>
       <c r="E40">
-        <v>9.8151960000000003</v>
+        <v>11.024823</v>
       </c>
       <c r="G40">
         <v>10.921894999999999</v>
       </c>
       <c r="J40">
         <f t="shared" si="1"/>
-        <v>1.3716491238630624</v>
+        <v>0.72054699999999983</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
-        <v>8.309238630624606E-4</v>
+        <v>0.51918797920899973</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
@@ -16400,18 +16604,21 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <v>9.8120130000000003</v>
+        <v>15.605622</v>
       </c>
       <c r="G41">
         <v>10.921894999999999</v>
       </c>
+      <c r="I41" t="s">
+        <v>125</v>
+      </c>
       <c r="J41">
         <f t="shared" si="1"/>
-        <v>0.69647245067556296</v>
+        <v>3.8018250000000364E-2</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
-        <v>0.13355425067556181</v>
+        <v>1.4453873330625277E-3</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -16425,22 +16632,26 @@
         <v>34</v>
       </c>
       <c r="E42">
-        <v>10.547658999999999</v>
+        <v>12.024711</v>
       </c>
       <c r="F42">
         <f>AVERAGE(E42:E45)</f>
-        <v>10.55297025</v>
+        <v>11.302342999999999</v>
       </c>
       <c r="G42">
         <v>9.3817959999999996</v>
       </c>
+      <c r="I42">
+        <f>I33-I35</f>
+        <v>0.80868187499999955</v>
+      </c>
       <c r="J42">
-        <f>(J14-I14)^2</f>
-        <v>4.678947532656233E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4112590000000003</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
-        <v>2.0059304753265619</v>
+        <v>1.9916519650810007</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
@@ -16454,18 +16665,21 @@
         <v>37</v>
       </c>
       <c r="E43">
-        <v>11.321642000000001</v>
+        <v>12.822445999999999</v>
       </c>
       <c r="G43">
         <v>9.3817959999999996</v>
       </c>
+      <c r="I43" t="s">
+        <v>126</v>
+      </c>
       <c r="J43">
-        <f>(J15-I15)^2</f>
-        <v>8.1302823632250068E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.52362325</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
-        <v>2.2056304236322481</v>
+        <v>2.3214278079405624</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
@@ -16479,18 +16693,22 @@
         <v>38</v>
       </c>
       <c r="E44">
-        <v>10.564242999999999</v>
+        <v>10.518284</v>
       </c>
       <c r="G44">
         <v>9.3817959999999996</v>
       </c>
+      <c r="I44">
+        <f>I37-I39</f>
+        <v>0.95018315625000049</v>
+      </c>
       <c r="J44">
-        <f t="shared" ref="J44:J49" si="3">(J16-I16)^2</f>
-        <v>0.57320684536806155</v>
+        <f t="shared" si="1"/>
+        <v>0.84799299999999889</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
-        <v>0.19615664536806243</v>
+        <v>0.71909212804899814</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -16504,18 +16722,18 @@
         <v>39</v>
       </c>
       <c r="E45">
-        <v>9.7783370000000005</v>
+        <v>9.8439309999999995</v>
       </c>
       <c r="G45">
         <v>9.3817959999999996</v>
       </c>
       <c r="J45">
-        <f t="shared" si="3"/>
-        <v>1.1578298006251252E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.1086682499999991</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
-        <v>1.4142911829800595</v>
+        <v>1.2291452885580605</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -16529,22 +16747,22 @@
         <v>34</v>
       </c>
       <c r="E46">
-        <v>11.832392</v>
+        <v>10.844619</v>
       </c>
       <c r="F46">
         <f>AVERAGE(E46:E49)</f>
-        <v>10.376536250000001</v>
+        <v>10.78000525</v>
       </c>
       <c r="G46">
         <v>9.5419870000000007</v>
       </c>
       <c r="J46">
-        <f t="shared" si="3"/>
-        <v>2.0786070189062561E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.8415597500000001</v>
       </c>
       <c r="L46">
         <f t="shared" si="2"/>
-        <v>1.8068030701890612</v>
+        <v>3.3913423128200626</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
@@ -16558,18 +16776,18 @@
         <v>37</v>
       </c>
       <c r="E47">
-        <v>10.246069</v>
+        <v>11.169124999999999</v>
       </c>
       <c r="G47">
         <v>9.5419870000000007</v>
       </c>
       <c r="J47">
-        <f t="shared" si="3"/>
-        <v>0.62008616448025289</v>
+        <f>ABS(K19-I19)</f>
+        <v>2.5134110000000014</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
-        <v>3.9499793644802548</v>
+        <v>6.3172348549210069</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
@@ -16583,21 +16801,21 @@
         <v>38</v>
       </c>
       <c r="E48">
-        <v>9.4793640000000003</v>
+        <v>11.242902000000001</v>
       </c>
       <c r="G48">
         <v>9.5419870000000007</v>
       </c>
       <c r="J48">
-        <f t="shared" si="3"/>
-        <v>1.9309832964030642</v>
+        <f t="shared" si="1"/>
+        <v>0.92305549999999847</v>
       </c>
       <c r="L48">
         <f t="shared" si="2"/>
-        <v>3.5947496403062995E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+        <v>0.85203145608024722</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -16608,21 +16826,21 @@
         <v>39</v>
       </c>
       <c r="E49">
-        <v>9.9483200000000007</v>
+        <v>9.8633749999999996</v>
       </c>
       <c r="G49">
         <v>9.5419870000000007</v>
       </c>
       <c r="J49">
-        <f t="shared" si="3"/>
-        <v>2.3217218765400616</v>
+        <f t="shared" si="1"/>
+        <v>0.20385925000000071</v>
       </c>
       <c r="L49">
         <f t="shared" si="2"/>
-        <v>0.10479447654006277</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+        <v>4.1558593810562788E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>107</v>
       </c>
@@ -16633,17 +16851,17 @@
         <v>34</v>
       </c>
       <c r="E50">
-        <v>8.7803909999999998</v>
+        <v>8.8404699999999998</v>
       </c>
       <c r="F50">
         <f>AVERAGE(E50:E53)</f>
-        <v>9.1393942500000005</v>
+        <v>9.144444</v>
       </c>
       <c r="G50">
         <v>9.3557030000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>107</v>
       </c>
@@ -16654,13 +16872,16 @@
         <v>37</v>
       </c>
       <c r="E51">
-        <v>9.1737330000000004</v>
+        <v>9.0955619999999993</v>
       </c>
       <c r="G51">
         <v>9.3557030000000001</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>107</v>
       </c>
@@ -16671,13 +16892,13 @@
         <v>38</v>
       </c>
       <c r="E52">
-        <v>9.2776730000000001</v>
+        <v>9.5807540000000007</v>
       </c>
       <c r="G52">
         <v>9.3557030000000001</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>107</v>
       </c>
@@ -16688,13 +16909,13 @@
         <v>39</v>
       </c>
       <c r="E53">
-        <v>9.32578</v>
+        <v>9.0609900000000003</v>
       </c>
       <c r="G53">
         <v>9.3557030000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>107</v>
       </c>
@@ -16705,17 +16926,17 @@
         <v>34</v>
       </c>
       <c r="E54">
-        <v>10.041607000000001</v>
+        <v>10.067997</v>
       </c>
       <c r="F54">
         <f>AVERAGE(E54:E57)</f>
-        <v>10.002458499999999</v>
+        <v>9.9639717499999989</v>
       </c>
       <c r="G54">
         <v>10.287595</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>107</v>
       </c>
@@ -16726,13 +16947,13 @@
         <v>37</v>
       </c>
       <c r="E55">
-        <v>9.8198120000000007</v>
+        <v>9.8091799999999996</v>
       </c>
       <c r="G55">
         <v>10.287595</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>107</v>
       </c>
@@ -16743,13 +16964,13 @@
         <v>38</v>
       </c>
       <c r="E56">
-        <v>10.293556000000001</v>
+        <v>10.21631</v>
       </c>
       <c r="G56">
         <v>10.287595</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>107</v>
       </c>
@@ -16760,13 +16981,13 @@
         <v>39</v>
       </c>
       <c r="E57">
-        <v>9.8548589999999994</v>
+        <v>9.7623999999999995</v>
       </c>
       <c r="G57">
         <v>10.287595</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>108</v>
       </c>
@@ -16777,17 +16998,17 @@
         <v>34</v>
       </c>
       <c r="E58">
-        <v>10.363528000000001</v>
+        <v>10.416802000000001</v>
       </c>
       <c r="F58">
         <f>AVERAGE(E58:E61)</f>
-        <v>10.573042249999999</v>
+        <v>10.167945</v>
       </c>
       <c r="G58">
         <v>9.8159379999999992</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>108</v>
       </c>
@@ -16798,13 +17019,13 @@
         <v>37</v>
       </c>
       <c r="E59">
-        <v>9.9679210000000005</v>
+        <v>10.005442</v>
       </c>
       <c r="G59">
         <v>9.8159379999999992</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>108</v>
       </c>
@@ -16815,13 +17036,13 @@
         <v>38</v>
       </c>
       <c r="E60">
-        <v>11.168996999999999</v>
+        <v>10.017773999999999</v>
       </c>
       <c r="G60">
         <v>9.8159379999999992</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>108</v>
       </c>
@@ -16832,13 +17053,13 @@
         <v>39</v>
       </c>
       <c r="E61">
-        <v>10.791722999999999</v>
+        <v>10.231762</v>
       </c>
       <c r="G61">
         <v>9.8159379999999992</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>108</v>
       </c>
@@ -16849,17 +17070,17 @@
         <v>34</v>
       </c>
       <c r="E62">
-        <v>11.357813</v>
+        <v>11.607441</v>
       </c>
       <c r="F62">
         <f>AVERAGE(E62:E65)</f>
-        <v>11.120386250000001</v>
+        <v>11.200957750000001</v>
       </c>
       <c r="G62">
         <v>11.109626</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>108</v>
       </c>
@@ -16870,13 +17091,13 @@
         <v>37</v>
       </c>
       <c r="E63">
-        <v>10.975279</v>
+        <v>10.917972000000001</v>
       </c>
       <c r="G63">
         <v>11.109626</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>108</v>
       </c>
@@ -16887,7 +17108,7 @@
         <v>38</v>
       </c>
       <c r="E64">
-        <v>11.072824000000001</v>
+        <v>11.177757</v>
       </c>
       <c r="G64">
         <v>11.109626</v>
@@ -16904,7 +17125,7 @@
         <v>39</v>
       </c>
       <c r="E65">
-        <v>11.075628999999999</v>
+        <v>11.100661000000001</v>
       </c>
       <c r="G65">
         <v>11.109626</v>
@@ -16921,11 +17142,11 @@
         <v>34</v>
       </c>
       <c r="E66">
-        <v>11.109363</v>
+        <v>10.153517000000001</v>
       </c>
       <c r="F66">
         <f>AVERAGE(E66:E69)</f>
-        <v>11.10910825</v>
+        <v>10.61172225</v>
       </c>
       <c r="G66">
         <v>11.253282</v>
@@ -16942,7 +17163,7 @@
         <v>37</v>
       </c>
       <c r="E67">
-        <v>11.107533</v>
+        <v>10.576657000000001</v>
       </c>
       <c r="G67">
         <v>11.253282</v>
@@ -16959,7 +17180,7 @@
         <v>38</v>
       </c>
       <c r="E68">
-        <v>11.141007</v>
+        <v>10.638185</v>
       </c>
       <c r="G68">
         <v>11.253282</v>
@@ -16993,11 +17214,11 @@
         <v>34</v>
       </c>
       <c r="E70">
-        <v>11.145773999999999</v>
+        <v>10.981242999999999</v>
       </c>
       <c r="F70">
         <f>AVERAGE(E70:E73)</f>
-        <v>11.509599499999998</v>
+        <v>10.983643999999998</v>
       </c>
       <c r="G70">
         <v>12.297055</v>
@@ -17014,7 +17235,7 @@
         <v>37</v>
       </c>
       <c r="E71">
-        <v>11.527557</v>
+        <v>11.491835999999999</v>
       </c>
       <c r="G71">
         <v>12.297055</v>
@@ -17031,7 +17252,7 @@
         <v>38</v>
       </c>
       <c r="E72">
-        <v>11.008775999999999</v>
+        <v>10.333209</v>
       </c>
       <c r="G72">
         <v>12.297055</v>
@@ -17048,7 +17269,7 @@
         <v>39</v>
       </c>
       <c r="E73">
-        <v>12.356291000000001</v>
+        <v>11.128288</v>
       </c>
       <c r="G73">
         <v>12.297055</v>
@@ -17065,11 +17286,11 @@
         <v>34</v>
       </c>
       <c r="E74">
-        <v>11.589969</v>
+        <v>10.296685999999999</v>
       </c>
       <c r="F74">
         <f>AVERAGE(E74:E77)</f>
-        <v>11.507214250000001</v>
+        <v>10.394560500000001</v>
       </c>
       <c r="G74">
         <v>10.117616</v>
@@ -17086,7 +17307,7 @@
         <v>37</v>
       </c>
       <c r="E75">
-        <v>11.70552</v>
+        <v>10.624772</v>
       </c>
       <c r="G75">
         <v>10.117616</v>
@@ -17103,7 +17324,7 @@
         <v>38</v>
       </c>
       <c r="E76">
-        <v>11.39451</v>
+        <v>10.236551</v>
       </c>
       <c r="G76">
         <v>10.117616</v>
@@ -17120,7 +17341,7 @@
         <v>39</v>
       </c>
       <c r="E77">
-        <v>11.338858</v>
+        <v>10.420233</v>
       </c>
       <c r="G77">
         <v>10.117616</v>
@@ -17137,11 +17358,11 @@
         <v>34</v>
       </c>
       <c r="E78">
-        <v>12.432638000000001</v>
+        <v>12.651707</v>
       </c>
       <c r="F78">
         <f>AVERAGE(E78:E81)</f>
-        <v>12.46143575</v>
+        <v>12.34157525</v>
       </c>
       <c r="G78">
         <v>10.937716</v>
@@ -17158,7 +17379,7 @@
         <v>37</v>
       </c>
       <c r="E79">
-        <v>12.816719000000001</v>
+        <v>12.716286</v>
       </c>
       <c r="G79">
         <v>10.937716</v>
@@ -17175,13 +17396,13 @@
         <v>38</v>
       </c>
       <c r="E80">
-        <v>12.255646</v>
+        <v>11.931950000000001</v>
       </c>
       <c r="G80">
         <v>10.937716</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>110</v>
       </c>
@@ -17192,9 +17413,1289 @@
         <v>39</v>
       </c>
       <c r="E81">
-        <v>12.34074</v>
+        <v>12.066357999999999</v>
       </c>
       <c r="G81">
+        <v>10.937716</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86">
+        <v>10.006568</v>
+      </c>
+      <c r="F86">
+        <v>8.9729109999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" t="s">
+        <v>37</v>
+      </c>
+      <c r="E87">
+        <v>9.5207770000000007</v>
+      </c>
+      <c r="F87">
+        <v>8.9729109999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>33</v>
+      </c>
+      <c r="D88" t="s">
+        <v>38</v>
+      </c>
+      <c r="E88">
+        <v>10.042546</v>
+      </c>
+      <c r="F88">
+        <v>8.9729109999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
+        <v>43</v>
+      </c>
+      <c r="C89" t="s">
+        <v>33</v>
+      </c>
+      <c r="D89" t="s">
+        <v>39</v>
+      </c>
+      <c r="E89">
+        <v>9.5741569999999996</v>
+      </c>
+      <c r="F89">
+        <v>8.9729109999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>4</v>
+      </c>
+      <c r="B90" t="s">
+        <v>43</v>
+      </c>
+      <c r="C90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90">
+        <v>10.400014000000001</v>
+      </c>
+      <c r="F90">
+        <v>9.3905689999999993</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91" t="s">
+        <v>43</v>
+      </c>
+      <c r="C91" t="s">
+        <v>40</v>
+      </c>
+      <c r="D91" t="s">
+        <v>37</v>
+      </c>
+      <c r="E91">
+        <v>11.22617</v>
+      </c>
+      <c r="F91">
+        <v>9.3905689999999993</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>43</v>
+      </c>
+      <c r="C92" t="s">
+        <v>40</v>
+      </c>
+      <c r="D92" t="s">
+        <v>38</v>
+      </c>
+      <c r="E92">
+        <v>10.226703000000001</v>
+      </c>
+      <c r="F92">
+        <v>9.3905689999999993</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>7</v>
+      </c>
+      <c r="B93" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" t="s">
+        <v>40</v>
+      </c>
+      <c r="D93" t="s">
+        <v>39</v>
+      </c>
+      <c r="E93">
+        <v>10.292716</v>
+      </c>
+      <c r="F93">
+        <v>9.3905689999999993</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>8</v>
+      </c>
+      <c r="B94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94">
+        <v>10.827400000000001</v>
+      </c>
+      <c r="F94">
+        <v>9.5206529999999994</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>44</v>
+      </c>
+      <c r="C95" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>37</v>
+      </c>
+      <c r="E95">
+        <v>10.524960999999999</v>
+      </c>
+      <c r="F95">
+        <v>9.5206529999999994</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>10</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" t="s">
+        <v>38</v>
+      </c>
+      <c r="E96">
+        <v>10.395058000000001</v>
+      </c>
+      <c r="F96">
+        <v>9.5206529999999994</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>11</v>
+      </c>
+      <c r="B97" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" t="s">
+        <v>39</v>
+      </c>
+      <c r="E97">
+        <v>11.132913</v>
+      </c>
+      <c r="F97">
+        <v>9.5206529999999994</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98" t="s">
+        <v>40</v>
+      </c>
+      <c r="D98" t="s">
+        <v>34</v>
+      </c>
+      <c r="E98">
+        <v>11.04608</v>
+      </c>
+      <c r="F98">
+        <v>9.8293160000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>13</v>
+      </c>
+      <c r="B99" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" t="s">
+        <v>37</v>
+      </c>
+      <c r="E99">
+        <v>11.047166000000001</v>
+      </c>
+      <c r="F99">
+        <v>9.8293160000000004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>14</v>
+      </c>
+      <c r="B100" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" t="s">
+        <v>38</v>
+      </c>
+      <c r="E100">
+        <v>11.052873</v>
+      </c>
+      <c r="F100">
+        <v>9.8293160000000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>15</v>
+      </c>
+      <c r="B101" t="s">
+        <v>44</v>
+      </c>
+      <c r="C101" t="s">
+        <v>40</v>
+      </c>
+      <c r="D101" t="s">
+        <v>39</v>
+      </c>
+      <c r="E101">
+        <v>11.209542000000001</v>
+      </c>
+      <c r="F101">
+        <v>9.8293160000000004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>16</v>
+      </c>
+      <c r="B102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C102" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" t="s">
+        <v>34</v>
+      </c>
+      <c r="E102">
+        <v>9.1992360000000009</v>
+      </c>
+      <c r="F102">
+        <v>9.4284049999999997</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>17</v>
+      </c>
+      <c r="B103" t="s">
+        <v>105</v>
+      </c>
+      <c r="C103" t="s">
+        <v>33</v>
+      </c>
+      <c r="D103" t="s">
+        <v>37</v>
+      </c>
+      <c r="E103">
+        <v>9.1908220000000007</v>
+      </c>
+      <c r="F103">
+        <v>9.4284049999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>18</v>
+      </c>
+      <c r="B104" t="s">
+        <v>105</v>
+      </c>
+      <c r="C104" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" t="s">
+        <v>38</v>
+      </c>
+      <c r="E104">
+        <v>11.342254000000001</v>
+      </c>
+      <c r="F104">
+        <v>9.4284049999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>19</v>
+      </c>
+      <c r="B105" t="s">
+        <v>105</v>
+      </c>
+      <c r="C105" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" t="s">
+        <v>39</v>
+      </c>
+      <c r="E105">
+        <v>9.6051350000000006</v>
+      </c>
+      <c r="F105">
+        <v>9.4284049999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>20</v>
+      </c>
+      <c r="B106" t="s">
+        <v>105</v>
+      </c>
+      <c r="C106" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" t="s">
+        <v>34</v>
+      </c>
+      <c r="E106">
+        <v>10.902462</v>
+      </c>
+      <c r="F106">
+        <v>10.921894999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>21</v>
+      </c>
+      <c r="B107" t="s">
+        <v>105</v>
+      </c>
+      <c r="C107" t="s">
+        <v>40</v>
+      </c>
+      <c r="D107" t="s">
+        <v>37</v>
+      </c>
+      <c r="E107">
+        <v>13.13696</v>
+      </c>
+      <c r="F107">
+        <v>10.921894999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>22</v>
+      </c>
+      <c r="B108" t="s">
+        <v>105</v>
+      </c>
+      <c r="C108" t="s">
+        <v>40</v>
+      </c>
+      <c r="D108" t="s">
+        <v>38</v>
+      </c>
+      <c r="E108">
+        <v>11.024823</v>
+      </c>
+      <c r="F108">
+        <v>10.921894999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>23</v>
+      </c>
+      <c r="B109" t="s">
+        <v>105</v>
+      </c>
+      <c r="C109" t="s">
+        <v>40</v>
+      </c>
+      <c r="D109" t="s">
+        <v>39</v>
+      </c>
+      <c r="E109">
+        <v>15.605622</v>
+      </c>
+      <c r="F109">
+        <v>10.921894999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
+        <v>106</v>
+      </c>
+      <c r="C110" t="s">
+        <v>33</v>
+      </c>
+      <c r="D110" t="s">
+        <v>34</v>
+      </c>
+      <c r="E110">
+        <v>12.024711</v>
+      </c>
+      <c r="F110">
+        <v>9.3817959999999996</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>25</v>
+      </c>
+      <c r="B111" t="s">
+        <v>106</v>
+      </c>
+      <c r="C111" t="s">
+        <v>33</v>
+      </c>
+      <c r="D111" t="s">
+        <v>37</v>
+      </c>
+      <c r="E111">
+        <v>12.822445999999999</v>
+      </c>
+      <c r="F111">
+        <v>9.3817959999999996</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>26</v>
+      </c>
+      <c r="B112" t="s">
+        <v>106</v>
+      </c>
+      <c r="C112" t="s">
+        <v>33</v>
+      </c>
+      <c r="D112" t="s">
+        <v>38</v>
+      </c>
+      <c r="E112">
+        <v>10.518284</v>
+      </c>
+      <c r="F112">
+        <v>9.3817959999999996</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>27</v>
+      </c>
+      <c r="B113" t="s">
+        <v>106</v>
+      </c>
+      <c r="C113" t="s">
+        <v>33</v>
+      </c>
+      <c r="D113" t="s">
+        <v>39</v>
+      </c>
+      <c r="E113">
+        <v>9.8439309999999995</v>
+      </c>
+      <c r="F113">
+        <v>9.3817959999999996</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>28</v>
+      </c>
+      <c r="B114" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114" t="s">
+        <v>40</v>
+      </c>
+      <c r="D114" t="s">
+        <v>34</v>
+      </c>
+      <c r="E114">
+        <v>10.844619</v>
+      </c>
+      <c r="F114">
+        <v>9.5419870000000007</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>29</v>
+      </c>
+      <c r="B115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C115" t="s">
+        <v>40</v>
+      </c>
+      <c r="D115" t="s">
+        <v>37</v>
+      </c>
+      <c r="E115">
+        <v>11.169124999999999</v>
+      </c>
+      <c r="F115">
+        <v>9.5419870000000007</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>30</v>
+      </c>
+      <c r="B116" t="s">
+        <v>106</v>
+      </c>
+      <c r="C116" t="s">
+        <v>40</v>
+      </c>
+      <c r="D116" t="s">
+        <v>38</v>
+      </c>
+      <c r="E116">
+        <v>11.242902000000001</v>
+      </c>
+      <c r="F116">
+        <v>9.5419870000000007</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>31</v>
+      </c>
+      <c r="B117" t="s">
+        <v>106</v>
+      </c>
+      <c r="C117" t="s">
+        <v>40</v>
+      </c>
+      <c r="D117" t="s">
+        <v>39</v>
+      </c>
+      <c r="E117">
+        <v>9.8633749999999996</v>
+      </c>
+      <c r="F117">
+        <v>9.5419870000000007</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>32</v>
+      </c>
+      <c r="B118" t="s">
+        <v>107</v>
+      </c>
+      <c r="C118" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118" t="s">
+        <v>34</v>
+      </c>
+      <c r="E118">
+        <v>8.8404699999999998</v>
+      </c>
+      <c r="F118">
+        <v>9.3557030000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>33</v>
+      </c>
+      <c r="B119" t="s">
+        <v>107</v>
+      </c>
+      <c r="C119" t="s">
+        <v>33</v>
+      </c>
+      <c r="D119" t="s">
+        <v>37</v>
+      </c>
+      <c r="E119">
+        <v>9.0955619999999993</v>
+      </c>
+      <c r="F119">
+        <v>9.3557030000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>34</v>
+      </c>
+      <c r="B120" t="s">
+        <v>107</v>
+      </c>
+      <c r="C120" t="s">
+        <v>33</v>
+      </c>
+      <c r="D120" t="s">
+        <v>38</v>
+      </c>
+      <c r="E120">
+        <v>9.5807540000000007</v>
+      </c>
+      <c r="F120">
+        <v>9.3557030000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>35</v>
+      </c>
+      <c r="B121" t="s">
+        <v>107</v>
+      </c>
+      <c r="C121" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" t="s">
+        <v>39</v>
+      </c>
+      <c r="E121">
+        <v>9.0609900000000003</v>
+      </c>
+      <c r="F121">
+        <v>9.3557030000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>36</v>
+      </c>
+      <c r="B122" t="s">
+        <v>107</v>
+      </c>
+      <c r="C122" t="s">
+        <v>40</v>
+      </c>
+      <c r="D122" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122">
+        <v>10.067997</v>
+      </c>
+      <c r="F122">
+        <v>10.287595</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>37</v>
+      </c>
+      <c r="B123" t="s">
+        <v>107</v>
+      </c>
+      <c r="C123" t="s">
+        <v>40</v>
+      </c>
+      <c r="D123" t="s">
+        <v>37</v>
+      </c>
+      <c r="E123">
+        <v>9.8091799999999996</v>
+      </c>
+      <c r="F123">
+        <v>10.287595</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>38</v>
+      </c>
+      <c r="B124" t="s">
+        <v>107</v>
+      </c>
+      <c r="C124" t="s">
+        <v>40</v>
+      </c>
+      <c r="D124" t="s">
+        <v>38</v>
+      </c>
+      <c r="E124">
+        <v>10.21631</v>
+      </c>
+      <c r="F124">
+        <v>10.287595</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>39</v>
+      </c>
+      <c r="B125" t="s">
+        <v>107</v>
+      </c>
+      <c r="C125" t="s">
+        <v>40</v>
+      </c>
+      <c r="D125" t="s">
+        <v>39</v>
+      </c>
+      <c r="E125">
+        <v>9.7623999999999995</v>
+      </c>
+      <c r="F125">
+        <v>10.287595</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>40</v>
+      </c>
+      <c r="B126" t="s">
+        <v>108</v>
+      </c>
+      <c r="C126" t="s">
+        <v>33</v>
+      </c>
+      <c r="D126" t="s">
+        <v>34</v>
+      </c>
+      <c r="E126">
+        <v>10.416802000000001</v>
+      </c>
+      <c r="F126">
+        <v>9.8159379999999992</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>41</v>
+      </c>
+      <c r="B127" t="s">
+        <v>108</v>
+      </c>
+      <c r="C127" t="s">
+        <v>33</v>
+      </c>
+      <c r="D127" t="s">
+        <v>37</v>
+      </c>
+      <c r="E127">
+        <v>10.005442</v>
+      </c>
+      <c r="F127">
+        <v>9.8159379999999992</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>42</v>
+      </c>
+      <c r="B128" t="s">
+        <v>108</v>
+      </c>
+      <c r="C128" t="s">
+        <v>33</v>
+      </c>
+      <c r="D128" t="s">
+        <v>38</v>
+      </c>
+      <c r="E128">
+        <v>10.017773999999999</v>
+      </c>
+      <c r="F128">
+        <v>9.8159379999999992</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>43</v>
+      </c>
+      <c r="B129" t="s">
+        <v>108</v>
+      </c>
+      <c r="C129" t="s">
+        <v>33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>39</v>
+      </c>
+      <c r="E129">
+        <v>10.231762</v>
+      </c>
+      <c r="F129">
+        <v>9.8159379999999992</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>44</v>
+      </c>
+      <c r="B130" t="s">
+        <v>108</v>
+      </c>
+      <c r="C130" t="s">
+        <v>40</v>
+      </c>
+      <c r="D130" t="s">
+        <v>34</v>
+      </c>
+      <c r="E130">
+        <v>11.607441</v>
+      </c>
+      <c r="F130">
+        <v>11.109626</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>45</v>
+      </c>
+      <c r="B131" t="s">
+        <v>108</v>
+      </c>
+      <c r="C131" t="s">
+        <v>40</v>
+      </c>
+      <c r="D131" t="s">
+        <v>37</v>
+      </c>
+      <c r="E131">
+        <v>10.917972000000001</v>
+      </c>
+      <c r="F131">
+        <v>11.109626</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>46</v>
+      </c>
+      <c r="B132" t="s">
+        <v>108</v>
+      </c>
+      <c r="C132" t="s">
+        <v>40</v>
+      </c>
+      <c r="D132" t="s">
+        <v>38</v>
+      </c>
+      <c r="E132">
+        <v>11.177757</v>
+      </c>
+      <c r="F132">
+        <v>11.109626</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>47</v>
+      </c>
+      <c r="B133" t="s">
+        <v>108</v>
+      </c>
+      <c r="C133" t="s">
+        <v>40</v>
+      </c>
+      <c r="D133" t="s">
+        <v>39</v>
+      </c>
+      <c r="E133">
+        <v>11.100661000000001</v>
+      </c>
+      <c r="F133">
+        <v>11.109626</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>48</v>
+      </c>
+      <c r="B134" t="s">
+        <v>109</v>
+      </c>
+      <c r="C134" t="s">
+        <v>33</v>
+      </c>
+      <c r="D134" t="s">
+        <v>34</v>
+      </c>
+      <c r="E134">
+        <v>10.153517000000001</v>
+      </c>
+      <c r="F134">
+        <v>11.253282</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>49</v>
+      </c>
+      <c r="B135" t="s">
+        <v>109</v>
+      </c>
+      <c r="C135" t="s">
+        <v>33</v>
+      </c>
+      <c r="D135" t="s">
+        <v>37</v>
+      </c>
+      <c r="E135">
+        <v>10.576657000000001</v>
+      </c>
+      <c r="F135">
+        <v>11.253282</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>50</v>
+      </c>
+      <c r="B136" t="s">
+        <v>109</v>
+      </c>
+      <c r="C136" t="s">
+        <v>33</v>
+      </c>
+      <c r="D136" t="s">
+        <v>38</v>
+      </c>
+      <c r="E136">
+        <v>10.638185</v>
+      </c>
+      <c r="F136">
+        <v>11.253282</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>51</v>
+      </c>
+      <c r="B137" t="s">
+        <v>109</v>
+      </c>
+      <c r="C137" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" t="s">
+        <v>39</v>
+      </c>
+      <c r="E137">
+        <v>11.078530000000001</v>
+      </c>
+      <c r="F137">
+        <v>11.253282</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>52</v>
+      </c>
+      <c r="B138" t="s">
+        <v>109</v>
+      </c>
+      <c r="C138" t="s">
+        <v>40</v>
+      </c>
+      <c r="D138" t="s">
+        <v>34</v>
+      </c>
+      <c r="E138">
+        <v>10.981242999999999</v>
+      </c>
+      <c r="F138">
+        <v>12.297055</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>53</v>
+      </c>
+      <c r="B139" t="s">
+        <v>109</v>
+      </c>
+      <c r="C139" t="s">
+        <v>40</v>
+      </c>
+      <c r="D139" t="s">
+        <v>37</v>
+      </c>
+      <c r="E139">
+        <v>11.491835999999999</v>
+      </c>
+      <c r="F139">
+        <v>12.297055</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>54</v>
+      </c>
+      <c r="B140" t="s">
+        <v>109</v>
+      </c>
+      <c r="C140" t="s">
+        <v>40</v>
+      </c>
+      <c r="D140" t="s">
+        <v>38</v>
+      </c>
+      <c r="E140">
+        <v>10.333209</v>
+      </c>
+      <c r="F140">
+        <v>12.297055</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>55</v>
+      </c>
+      <c r="B141" t="s">
+        <v>109</v>
+      </c>
+      <c r="C141" t="s">
+        <v>40</v>
+      </c>
+      <c r="D141" t="s">
+        <v>39</v>
+      </c>
+      <c r="E141">
+        <v>11.128288</v>
+      </c>
+      <c r="F141">
+        <v>12.297055</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>56</v>
+      </c>
+      <c r="B142" t="s">
+        <v>110</v>
+      </c>
+      <c r="C142" t="s">
+        <v>33</v>
+      </c>
+      <c r="D142" t="s">
+        <v>34</v>
+      </c>
+      <c r="E142">
+        <v>10.296685999999999</v>
+      </c>
+      <c r="F142">
+        <v>10.117616</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>57</v>
+      </c>
+      <c r="B143" t="s">
+        <v>110</v>
+      </c>
+      <c r="C143" t="s">
+        <v>33</v>
+      </c>
+      <c r="D143" t="s">
+        <v>37</v>
+      </c>
+      <c r="E143">
+        <v>10.624772</v>
+      </c>
+      <c r="F143">
+        <v>10.117616</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>58</v>
+      </c>
+      <c r="B144" t="s">
+        <v>110</v>
+      </c>
+      <c r="C144" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144" t="s">
+        <v>38</v>
+      </c>
+      <c r="E144">
+        <v>10.236551</v>
+      </c>
+      <c r="F144">
+        <v>10.117616</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>59</v>
+      </c>
+      <c r="B145" t="s">
+        <v>110</v>
+      </c>
+      <c r="C145" t="s">
+        <v>33</v>
+      </c>
+      <c r="D145" t="s">
+        <v>39</v>
+      </c>
+      <c r="E145">
+        <v>10.420233</v>
+      </c>
+      <c r="F145">
+        <v>10.117616</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>60</v>
+      </c>
+      <c r="B146" t="s">
+        <v>110</v>
+      </c>
+      <c r="C146" t="s">
+        <v>40</v>
+      </c>
+      <c r="D146" t="s">
+        <v>34</v>
+      </c>
+      <c r="E146">
+        <v>12.651707</v>
+      </c>
+      <c r="F146">
+        <v>10.937716</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>61</v>
+      </c>
+      <c r="B147" t="s">
+        <v>110</v>
+      </c>
+      <c r="C147" t="s">
+        <v>40</v>
+      </c>
+      <c r="D147" t="s">
+        <v>37</v>
+      </c>
+      <c r="E147">
+        <v>12.716286</v>
+      </c>
+      <c r="F147">
+        <v>10.937716</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>62</v>
+      </c>
+      <c r="B148" t="s">
+        <v>110</v>
+      </c>
+      <c r="C148" t="s">
+        <v>40</v>
+      </c>
+      <c r="D148" t="s">
+        <v>38</v>
+      </c>
+      <c r="E148">
+        <v>11.931950000000001</v>
+      </c>
+      <c r="F148">
+        <v>10.937716</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>63</v>
+      </c>
+      <c r="B149" t="s">
+        <v>110</v>
+      </c>
+      <c r="C149" t="s">
+        <v>40</v>
+      </c>
+      <c r="D149" t="s">
+        <v>39</v>
+      </c>
+      <c r="E149">
+        <v>12.066357999999999</v>
+      </c>
+      <c r="F149">
         <v>10.937716</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final paper updates/tweaks. Generally same.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons_rev2.xlsx
+++ b/metaboliccostcomparisons_rev2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC12FC50-C82D-4693-B51E-760D90A87A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C856C-943D-4246-A9E7-3207CEF5FDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="573" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="573" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fullcost t test" sheetId="5" r:id="rId1"/>
     <sheet name="swing t test" sheetId="1" r:id="rId2"/>
     <sheet name="stance t test" sheetId="8" r:id="rId3"/>
-    <sheet name="100con_no_007" sheetId="11" r:id="rId4"/>
-    <sheet name="plusminuses" sheetId="12" r:id="rId5"/>
+    <sheet name="plusminuses" sheetId="12" r:id="rId4"/>
+    <sheet name="100con_no_007" sheetId="11" r:id="rId5"/>
     <sheet name="100con" sheetId="9" r:id="rId6"/>
     <sheet name="alldata_1step" sheetId="4" r:id="rId7"/>
     <sheet name="prescribe" sheetId="10" r:id="rId8"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="229">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -710,6 +710,24 @@
   </si>
   <si>
     <t>stance percent (exo-nat)/whole body nat</t>
+  </si>
+  <si>
+    <t>Stance percent change - respect to itself</t>
+  </si>
+  <si>
+    <t>exo-natural / natural*100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard error </t>
+  </si>
+  <si>
+    <t>Average of ones we want</t>
+  </si>
+  <si>
+    <t>SE ones we want</t>
+  </si>
+  <si>
+    <t>std ones that we want</t>
   </si>
 </sst>
 </file>
@@ -2794,49 +2812,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Experimental vs Simulated Cost</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12332327600819439"/>
-          <c:y val="9.4695698727498591E-3"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2844,9 +2820,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.14312872033260451"/>
-          <c:y val="0.12998177667026062"/>
-          <c:w val="0.64115461804755236"/>
-          <c:h val="0.68248395516842164"/>
+          <c:y val="0.12236625710091925"/>
+          <c:w val="0.61170716514775136"/>
+          <c:h val="0.69009955528669864"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3324,13 +3300,14 @@
           </c:spPr>
           <c:trendline>
             <c:spPr>
-              <a:ln>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:alpha val="39000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
               </a:ln>
+              <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
@@ -3799,7 +3776,8 @@
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -3807,9 +3785,10 @@
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Simulated Cost [W/kg]</a:t>
+                  <a:t>Simulated Cost (W/kg)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3823,7 +3802,7 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3843,7 +3822,8 @@
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3882,7 +3862,8 @@
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -3890,9 +3871,10 @@
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Experimental Cost [W/kg]</a:t>
+                  <a:t>Measured Cost (W/kg)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3914,7 +3896,7 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3934,7 +3916,8 @@
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3961,11 +3944,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3980,10 +3964,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78239874469084636"/>
-          <c:y val="0.23045689556182883"/>
-          <c:w val="0.21760125530915378"/>
-          <c:h val="0.56406226155200534"/>
+          <c:x val="0.76001868682657558"/>
+          <c:y val="0.23350308658447208"/>
+          <c:w val="0.19683540799339488"/>
+          <c:h val="0.43690576275217829"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3998,11 +3982,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2400" b="0" strike="noStrike" spc="-1">
+            <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -43161,12 +43146,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.42658</cdr:x>
-      <cdr:y>0.65473</cdr:y>
+      <cdr:x>0.41157</cdr:x>
+      <cdr:y>0.65584</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.55711</cdr:x>
-      <cdr:y>0.69903</cdr:y>
+      <cdr:x>0.53733</cdr:x>
+      <cdr:y>0.69884</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43181,8 +43166,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="4599637" y="5315486"/>
-          <a:ext cx="1407422" cy="359598"/>
+          <a:off x="4437530" y="5468471"/>
+          <a:ext cx="1355912" cy="358588"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -43214,12 +43199,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.39134</cdr:x>
-      <cdr:y>0.6079</cdr:y>
+      <cdr:x>0.37416</cdr:x>
+      <cdr:y>0.60342</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.45265</cdr:x>
-      <cdr:y>0.63578</cdr:y>
+      <cdr:x>0.44275</cdr:x>
+      <cdr:y>0.63433</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43234,8 +43219,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="4219624" y="4935233"/>
-          <a:ext cx="661074" cy="226350"/>
+          <a:off x="4034118" y="5031441"/>
+          <a:ext cx="739588" cy="257735"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -43269,12 +43254,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.46182</cdr:x>
-      <cdr:y>0.48225</cdr:y>
+      <cdr:x>0.44587</cdr:x>
+      <cdr:y>0.47978</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.71067</cdr:x>
-      <cdr:y>0.57231</cdr:y>
+      <cdr:x>0.67972</cdr:x>
+      <cdr:y>0.56848</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43289,8 +43274,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="4979650" y="3915180"/>
-          <a:ext cx="2683167" cy="731133"/>
+          <a:off x="4807324" y="4000500"/>
+          <a:ext cx="2521324" cy="739588"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -43322,12 +43307,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.37315</cdr:x>
-      <cdr:y>0.45775</cdr:y>
+      <cdr:x>0.36272</cdr:x>
+      <cdr:y>0.45693</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.52636</cdr:x>
-      <cdr:y>0.60364</cdr:y>
+      <cdr:x>0.50511</cdr:x>
+      <cdr:y>0.59939</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43342,8 +43327,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="4023564" y="3716230"/>
-          <a:ext cx="1651954" cy="1184456"/>
+          <a:off x="3910853" y="3810000"/>
+          <a:ext cx="1535206" cy="1187823"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -43375,12 +43360,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.29888</cdr:x>
-      <cdr:y>0.55136</cdr:y>
+      <cdr:x>0.29205</cdr:x>
+      <cdr:y>0.54698</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38356</cdr:x>
-      <cdr:y>0.65653</cdr:y>
+      <cdr:x>0.37416</cdr:x>
+      <cdr:y>0.65584</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43395,8 +43380,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="3222707" y="4476256"/>
-          <a:ext cx="913018" cy="853796"/>
+          <a:off x="3148853" y="4560794"/>
+          <a:ext cx="885265" cy="907677"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -43428,12 +43413,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.23068</cdr:x>
-      <cdr:y>0.48024</cdr:y>
+      <cdr:x>0.22345</cdr:x>
+      <cdr:y>0.47575</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.45908</cdr:x>
-      <cdr:y>0.64789</cdr:y>
+      <cdr:x>0.44483</cdr:x>
+      <cdr:y>0.64912</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43448,8 +43433,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="2487358" y="3898834"/>
-          <a:ext cx="2462681" cy="1361084"/>
+          <a:off x="2409265" y="3966882"/>
+          <a:ext cx="2386853" cy="1445559"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -43481,12 +43466,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.50823</cdr:x>
-      <cdr:y>0.3307</cdr:y>
+      <cdr:x>0.4916</cdr:x>
+      <cdr:y>0.32254</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.60646</cdr:x>
-      <cdr:y>0.43242</cdr:y>
+      <cdr:x>0.58618</cdr:x>
+      <cdr:y>0.42973</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -43501,8 +43486,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="5479971" y="2684767"/>
-          <a:ext cx="1059213" cy="825816"/>
+          <a:off x="5300405" y="2689412"/>
+          <a:ext cx="1019713" cy="893772"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -45108,7 +45093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -45125,6 +45110,7 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
@@ -45515,15 +45501,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
@@ -46526,10 +46512,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB71C57-F672-4F0F-AF5A-E40E874EA6E6}">
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:Y52"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34:V39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47041,7 +47027,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>R3-N3</f>
+        <f t="shared" ref="A19:A25" si="0">R3-N3</f>
         <v>-1.5603469999999993</v>
       </c>
       <c r="B19">
@@ -47066,7 +47052,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" ref="A20:A24" si="0">R4-N4</f>
+        <f t="shared" si="0"/>
         <v>-1.0352190000000006</v>
       </c>
       <c r="B20">
@@ -47269,7 +47255,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>R9-N9</f>
+        <f t="shared" si="0"/>
         <v>-2.5115430000000005</v>
       </c>
       <c r="B25">
@@ -47467,7 +47453,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="33" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>9</v>
       </c>
@@ -47488,7 +47474,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>9</v>
       </c>
@@ -47514,7 +47500,10 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="35" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>223</v>
+      </c>
       <c r="E35">
         <v>10</v>
       </c>
@@ -47540,7 +47529,10 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="36" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>224</v>
+      </c>
       <c r="E36">
         <v>10</v>
       </c>
@@ -47557,7 +47549,11 @@
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="37" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f>(R3-N3)/N3*100</f>
+        <v>-16.49087010578442</v>
+      </c>
       <c r="E37">
         <v>13</v>
       </c>
@@ -47574,7 +47570,11 @@
         <v>0.97899999999999998</v>
       </c>
     </row>
-    <row r="38" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" ref="B38:B43" si="1">(R4-N4)/N4*100</f>
+        <v>-12.448037431927554</v>
+      </c>
       <c r="E38">
         <v>13</v>
       </c>
@@ -47597,7 +47597,11 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="39" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>-20.624023928482419</v>
+      </c>
       <c r="O39" s="35" t="s">
         <v>190</v>
       </c>
@@ -47606,6 +47610,63 @@
       </c>
       <c r="V39">
         <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>-16.886613863185467</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>-17.806488020251717</v>
+      </c>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>-10.227670925746979</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>-25.633247227237426</v>
+      </c>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f>AVERAGE(B37:B43)</f>
+        <v>-17.159564500373712</v>
+      </c>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f>_xlfn.STDEV.P(B37:B43)</f>
+        <v>4.7055526199750757</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <f>B49/SQRT(COUNT(B37:B43))</f>
+        <v>1.7785317162260679</v>
       </c>
     </row>
   </sheetData>
@@ -47623,11 +47684,943 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1ABE7E-150E-4D46-958B-4C378FF29328}">
+  <dimension ref="A1:H53"/>
+  <sheetViews>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>11.061007999999999</v>
+      </c>
+      <c r="C2">
+        <v>9.4568924999999986</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>$B2-$B3</f>
+        <v>-0.21504700000000021</v>
+      </c>
+      <c r="F2">
+        <f>(B2-B3)/B3*100</f>
+        <v>-1.9071120174564617</v>
+      </c>
+      <c r="G2">
+        <f>C2-C3</f>
+        <v>-1.1394537500000013</v>
+      </c>
+      <c r="H2">
+        <f>(C2-C3)/C3*100</f>
+        <v>-10.753270260491925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>11.276054999999999</v>
+      </c>
+      <c r="C3">
+        <v>10.59634625</v>
+      </c>
+      <c r="D3" s="21">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f>B4-B5</f>
+        <v>-0.41765799999999942</v>
+      </c>
+      <c r="F3">
+        <f>(B4-B5)/B5*100</f>
+        <v>-4.4476325130031995</v>
+      </c>
+      <c r="G3">
+        <f>C4-C5</f>
+        <v>-1.3023895000000003</v>
+      </c>
+      <c r="H3">
+        <f>(C4-C5)/C5*100</f>
+        <v>-10.956040195717138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>8.9729109999999999</v>
+      </c>
+      <c r="C4">
+        <v>10.58502125</v>
+      </c>
+      <c r="D4" s="21">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f>B6-B7</f>
+        <v>-0.30866300000000102</v>
+      </c>
+      <c r="F4">
+        <f>(B6-B7)/B7*100</f>
+        <v>-3.1402286791878598</v>
+      </c>
+      <c r="G4">
+        <f>C6-C7</f>
+        <v>-0.69229400000000041</v>
+      </c>
+      <c r="H4">
+        <f>(C6-C7)/C7*100</f>
+        <v>-6.3208264476882619</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>9.3905689999999993</v>
+      </c>
+      <c r="C5">
+        <v>11.887410750000001</v>
+      </c>
+      <c r="D5" s="21">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>B8-B9</f>
+        <v>0.11609499999999962</v>
+      </c>
+      <c r="F5">
+        <f>(B8-B9)/B9*100</f>
+        <v>1.2885992899634173</v>
+      </c>
+      <c r="G5">
+        <f>C8-C9</f>
+        <v>-0.64127275000000061</v>
+      </c>
+      <c r="H5">
+        <f>(C8-C9)/C9*100</f>
+        <v>-6.1489278867575043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>9.5206529999999994</v>
+      </c>
+      <c r="C6">
+        <v>10.260292750000001</v>
+      </c>
+      <c r="D6" s="21">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f>B10-B11</f>
+        <v>-1.4934899999999995</v>
+      </c>
+      <c r="F6">
+        <f>(B10-B11)/B11*100</f>
+        <v>-13.674275389023604</v>
+      </c>
+      <c r="G6">
+        <f>C10-C11</f>
+        <v>-2.1598272500000011</v>
+      </c>
+      <c r="H6">
+        <f>(C10-C11)/C11*100</f>
+        <v>-19.701614790491924</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>9.8293160000000004</v>
+      </c>
+      <c r="C7">
+        <v>10.952586750000002</v>
+      </c>
+      <c r="D7" s="21">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <f>B12-B13</f>
+        <v>-0.16019100000000108</v>
+      </c>
+      <c r="F7">
+        <f>(B12-B13)/B13*100</f>
+        <v>-1.6788012811168269</v>
+      </c>
+      <c r="G7">
+        <f>C12-C13</f>
+        <v>0.85087324999999936</v>
+      </c>
+      <c r="H7">
+        <f>(C12-C13)/C13*100</f>
+        <v>8.2566998338346291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>9.1254899999999992</v>
+      </c>
+      <c r="C8">
+        <v>9.7877445000000005</v>
+      </c>
+      <c r="D8" s="21">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <f>B14-B15</f>
+        <v>-0.9318919999999995</v>
+      </c>
+      <c r="F8">
+        <f>(B14-B15)/B15*100</f>
+        <v>-9.058404806954389</v>
+      </c>
+      <c r="G8">
+        <f>C14-C15</f>
+        <v>-0.79258325000000163</v>
+      </c>
+      <c r="H8">
+        <f>(C14-C15)/C15*100</f>
+        <v>-7.7274152716978657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>9.0093949999999996</v>
+      </c>
+      <c r="C9">
+        <v>10.429017250000001</v>
+      </c>
+      <c r="D9" s="21">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <f>B16-B17</f>
+        <v>-1.2936880000000013</v>
+      </c>
+      <c r="F9">
+        <f>(B16-B17)/B17*100</f>
+        <v>-11.64474843707611</v>
+      </c>
+      <c r="G9">
+        <f>C16-C17</f>
+        <v>-1.4686440000000012</v>
+      </c>
+      <c r="H9">
+        <f>(C16-C17)/C17*100</f>
+        <v>-12.682308661961972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>9.4284049999999997</v>
+      </c>
+      <c r="C10">
+        <v>8.8028642500000007</v>
+      </c>
+      <c r="D10" s="21">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f>B18-B19</f>
+        <v>-1.0437729999999998</v>
+      </c>
+      <c r="F10">
+        <f>(B18-B19)/B19*100</f>
+        <v>-8.4879916370220343</v>
+      </c>
+      <c r="G10">
+        <f>C18-C19</f>
+        <v>-1.0508347499999982</v>
+      </c>
+      <c r="H10">
+        <f>(C18-C19)/C19*100</f>
+        <v>-8.4730079257860496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>10.921894999999999</v>
+      </c>
+      <c r="C11">
+        <v>10.962691500000002</v>
+      </c>
+      <c r="D11" s="21">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <f>B20-B21</f>
+        <v>-0.82010000000000005</v>
+      </c>
+      <c r="F11">
+        <f>(B20-B21)/B21*100</f>
+        <v>-7.4979090698643125</v>
+      </c>
+      <c r="G11">
+        <f>C20-C21</f>
+        <v>-2.3854830000000007</v>
+      </c>
+      <c r="H11">
+        <f>(C20-C21)/C21*100</f>
+        <v>-17.909158925886505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>9.3817959999999996</v>
+      </c>
+      <c r="C12">
+        <v>11.156119500000001</v>
+      </c>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>9.5419870000000007</v>
+      </c>
+      <c r="C13">
+        <v>10.305246250000001</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>9.3557030000000001</v>
+      </c>
+      <c r="C14">
+        <v>9.4641872500000002</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36">
+        <f>AVERAGE(E2:E11)</f>
+        <v>-0.65684070000000028</v>
+      </c>
+      <c r="F14" s="36">
+        <f>AVERAGE(F2:F11)</f>
+        <v>-6.0248504540741381</v>
+      </c>
+      <c r="G14" s="36">
+        <f>AVERAGE(G2:G11)</f>
+        <v>-1.0781909000000005</v>
+      </c>
+      <c r="H14" s="36">
+        <f>AVERAGE(H2:H11)</f>
+        <v>-9.2415870532644497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>10.287595</v>
+      </c>
+      <c r="C15">
+        <v>10.256770500000002</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>9.8159379999999992</v>
+      </c>
+      <c r="C16">
+        <v>10.111613500000001</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="36">
+        <f>_xlfn.STDEV.P(E2:E11)</f>
+        <v>0.50747297712490058</v>
+      </c>
+      <c r="F16" s="36">
+        <f>_xlfn.STDEV.P(F2:F11)</f>
+        <v>4.5571426681842135</v>
+      </c>
+      <c r="G16" s="36">
+        <f>_xlfn.STDEV.P(G2:G11)</f>
+        <v>0.8502260917791824</v>
+      </c>
+      <c r="H16" s="36">
+        <f>_xlfn.STDEV.P(H2:H11)</f>
+        <v>7.2716637751868829</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>11.109626</v>
+      </c>
+      <c r="C17">
+        <v>11.580257500000002</v>
+      </c>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>11.253282</v>
+      </c>
+      <c r="C18">
+        <v>11.351310500000002</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>12.297055</v>
+      </c>
+      <c r="C19">
+        <v>12.40214525</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="27">
+        <f>AVERAGE(E3:E4,E6,E8:E11)</f>
+        <v>-0.90132342857142866</v>
+      </c>
+      <c r="F19" s="27">
+        <f>AVERAGE(F3:F4,F6,F8:F11)</f>
+        <v>-8.2787415045902168</v>
+      </c>
+      <c r="G19" s="27">
+        <f>AVERAGE(G3:G4,G6,G8:G11)</f>
+        <v>-1.4074365357142862</v>
+      </c>
+      <c r="H19" s="27">
+        <f>AVERAGE(H3:H4,H6,H8:H11)</f>
+        <v>-11.967196031318531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>10.117616</v>
+      </c>
+      <c r="C20">
+        <v>10.934422250000001</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>10.937716</v>
+      </c>
+      <c r="C21">
+        <v>13.319905250000001</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="27">
+        <f>_xlfn.STDEV.P(E3:E4,E6,E8:E11)</f>
+        <v>0.39957359395945252</v>
+      </c>
+      <c r="F21" s="27">
+        <f>_xlfn.STDEV.P(F3:F4,F6,F8:F11)</f>
+        <v>3.4389545442921081</v>
+      </c>
+      <c r="G21" s="27">
+        <f>_xlfn.STDEV.P(G3:G4,G6,G8:G11)</f>
+        <v>0.60404424501591514</v>
+      </c>
+      <c r="H21" s="27">
+        <f>_xlfn.STDEV.P(H3:H4,H6,H8:H11)</f>
+        <v>4.7618807758293462</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f>E21/SQRT(COUNT(E8:E11,E6,E3:E4))</f>
+        <v>0.15102462286928742</v>
+      </c>
+      <c r="F23">
+        <f>F21/SQRT(COUNT(F8:F11,F6,F3:F4))</f>
+        <v>1.2998026420360538</v>
+      </c>
+      <c r="G23">
+        <f>G21/SQRT(COUNT(G8:G11,G6,G3:G4))</f>
+        <v>0.22830726474169688</v>
+      </c>
+      <c r="H23">
+        <f>H21/SQRT(COUNT(H8:H11,H6,H3:H4))</f>
+        <v>1.7998217579691089</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="G26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>9.3905689999999993</v>
+      </c>
+      <c r="C28">
+        <v>8.9729109999999999</v>
+      </c>
+      <c r="D28">
+        <v>11.887410750000001</v>
+      </c>
+      <c r="E28">
+        <v>10.58502125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>9.8293160000000004</v>
+      </c>
+      <c r="C29">
+        <v>9.5206529999999994</v>
+      </c>
+      <c r="D29">
+        <v>10.952586750000002</v>
+      </c>
+      <c r="E29">
+        <v>10.260292750000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>10.921894999999999</v>
+      </c>
+      <c r="C30">
+        <v>9.4284049999999997</v>
+      </c>
+      <c r="D30">
+        <v>10.962691500000002</v>
+      </c>
+      <c r="E30">
+        <v>8.8028642500000007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>10.287595</v>
+      </c>
+      <c r="C31">
+        <v>9.3557030000000001</v>
+      </c>
+      <c r="D31">
+        <v>10.256770500000002</v>
+      </c>
+      <c r="E31">
+        <v>9.4641872500000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>11.109626</v>
+      </c>
+      <c r="C32">
+        <v>9.8159379999999992</v>
+      </c>
+      <c r="D32">
+        <v>11.580257500000002</v>
+      </c>
+      <c r="E32">
+        <v>10.111613500000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>12.297055</v>
+      </c>
+      <c r="C33">
+        <v>11.253282</v>
+      </c>
+      <c r="D33">
+        <v>12.40214525</v>
+      </c>
+      <c r="E33">
+        <v>11.351310500000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>10.937716</v>
+      </c>
+      <c r="C34">
+        <v>10.117616</v>
+      </c>
+      <c r="D34">
+        <v>13.319905250000001</v>
+      </c>
+      <c r="E34">
+        <v>10.934422250000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>219</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="37"/>
+      <c r="F42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>10.681967428571427</v>
+      </c>
+      <c r="D43">
+        <v>9.7806439999999988</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>11.623109642857145</v>
+      </c>
+      <c r="G43">
+        <v>10.215673107142859</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>0.91077104346628623</v>
+      </c>
+      <c r="D44">
+        <v>0.55135559337266693</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>1.0517231529273505</v>
+      </c>
+      <c r="G44">
+        <v>0.75271164061995599</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>7</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>0.90022642372726802</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46">
+        <v>0.77480369522652626</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>5.5253463356738246</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49">
+        <v>5.7073656214696671</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>7.397762964505794E-4</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50">
+        <v>6.2590716172419164E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>1.9431802805153031</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51">
+        <v>1.9431802805153031</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>1.4795525929011588E-3</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>1.2518143234483833E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2.4469118511449697</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="1">
+        <v>2.4469118511449697</v>
+      </c>
+      <c r="G53" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA391E9-48A1-41F4-999A-C126E3EDA00F}">
   <dimension ref="A1:CR141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C98" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -51146,6 +52139,15 @@
         <f t="shared" si="4"/>
         <v>9.5014980024986514E-4</v>
       </c>
+      <c r="P43" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q43" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="R43" s="35" t="s">
+        <v>226</v>
+      </c>
       <c r="U43"/>
       <c r="V43" s="29"/>
     </row>
@@ -51185,6 +52187,18 @@
         <f t="shared" si="4"/>
         <v>8.7424001300250909E-2</v>
       </c>
+      <c r="P44" s="35">
+        <f>AVERAGE(P31,P32,P34,P36,P37,P38,P39)</f>
+        <v>-0.90132342857142866</v>
+      </c>
+      <c r="Q44" s="35">
+        <f>AVERAGE(Q31,Q32,Q34,Q36,Q37,Q38,Q39)</f>
+        <v>-1.4074365357142862</v>
+      </c>
+      <c r="R44" s="35">
+        <f>AVERAGE(R31,R32,R34,R36,R37,R38,R39)</f>
+        <v>-1.4074365357142862</v>
+      </c>
       <c r="U44"/>
       <c r="V44" s="29"/>
     </row>
@@ -51212,6 +52226,15 @@
         <f t="shared" si="4"/>
         <v>0.22149400879225134</v>
       </c>
+      <c r="P45" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q45" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="R45" s="35" t="s">
+        <v>228</v>
+      </c>
       <c r="U45"/>
       <c r="V45" s="29"/>
     </row>
@@ -51248,6 +52271,18 @@
         <f t="shared" si="4"/>
         <v>9.6095868122503189E-3</v>
       </c>
+      <c r="P46" s="35">
+        <f>_xlfn.STDEV.P(P31,P32,P34,P36:P39)</f>
+        <v>0.39957359395945252</v>
+      </c>
+      <c r="Q46" s="35">
+        <f>_xlfn.STDEV.P(Q31,Q32,Q34,Q36:Q39)</f>
+        <v>0.60404424501591514</v>
+      </c>
+      <c r="R46" s="35">
+        <f>_xlfn.STDEV.P(R31,R32,R34,R36:R39)</f>
+        <v>0.60404424501591514</v>
+      </c>
       <c r="U46"/>
       <c r="V46" s="29"/>
     </row>
@@ -51283,6 +52318,15 @@
         <f t="shared" si="4"/>
         <v>1.1043960645062488E-2</v>
       </c>
+      <c r="P47" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q47" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="R47" s="35" t="s">
+        <v>227</v>
+      </c>
       <c r="U47"/>
       <c r="V47" s="29"/>
     </row>
@@ -51316,6 +52360,18 @@
         <f t="shared" si="4"/>
         <v>0.66717245003906389</v>
       </c>
+      <c r="P48" s="35">
+        <f>P46/SQRT(COUNT(P31,P32,P34,P36:P39))</f>
+        <v>0.15102462286928742</v>
+      </c>
+      <c r="Q48" s="35">
+        <f>Q46/SQRT(COUNT(Q31,Q32,Q34,Q36:Q39))</f>
+        <v>0.22830726474169688</v>
+      </c>
+      <c r="R48" s="35">
+        <f>R46/SQRT(COUNT(R31,R32,R34,R36:R39))</f>
+        <v>0.22830726474169688</v>
+      </c>
       <c r="U48"/>
       <c r="V48" s="29"/>
     </row>
@@ -53175,938 +54231,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1ABE7E-150E-4D46-958B-4C378FF29328}">
-  <dimension ref="A1:H53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>11.061007999999999</v>
-      </c>
-      <c r="C2">
-        <v>9.4568924999999986</v>
-      </c>
-      <c r="D2" s="21">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>$B2-$B3</f>
-        <v>-0.21504700000000021</v>
-      </c>
-      <c r="F2">
-        <f>(B2-B3)/B3*100</f>
-        <v>-1.9071120174564617</v>
-      </c>
-      <c r="G2">
-        <f>C2-C3</f>
-        <v>-1.1394537500000013</v>
-      </c>
-      <c r="H2">
-        <f>(C2-C3)/C3*100</f>
-        <v>-10.753270260491925</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>11.276054999999999</v>
-      </c>
-      <c r="C3">
-        <v>10.59634625</v>
-      </c>
-      <c r="D3" s="21">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <f>B4-B5</f>
-        <v>-0.41765799999999942</v>
-      </c>
-      <c r="F3">
-        <f>(B4-B5)/B5*100</f>
-        <v>-4.4476325130031995</v>
-      </c>
-      <c r="G3">
-        <f>C4-C5</f>
-        <v>-1.3023895000000003</v>
-      </c>
-      <c r="H3">
-        <f>(C4-C5)/C5*100</f>
-        <v>-10.956040195717138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>8.9729109999999999</v>
-      </c>
-      <c r="C4">
-        <v>10.58502125</v>
-      </c>
-      <c r="D4" s="21">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <f>B6-B7</f>
-        <v>-0.30866300000000102</v>
-      </c>
-      <c r="F4">
-        <f>(B6-B7)/B7*100</f>
-        <v>-3.1402286791878598</v>
-      </c>
-      <c r="G4">
-        <f>C6-C7</f>
-        <v>-0.69229400000000041</v>
-      </c>
-      <c r="H4">
-        <f>(C6-C7)/C7*100</f>
-        <v>-6.3208264476882619</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>9.3905689999999993</v>
-      </c>
-      <c r="C5">
-        <v>11.887410750000001</v>
-      </c>
-      <c r="D5" s="21">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <f>B8-B9</f>
-        <v>0.11609499999999962</v>
-      </c>
-      <c r="F5">
-        <f>(B8-B9)/B9*100</f>
-        <v>1.2885992899634173</v>
-      </c>
-      <c r="G5">
-        <f>C8-C9</f>
-        <v>-0.64127275000000061</v>
-      </c>
-      <c r="H5">
-        <f>(C8-C9)/C9*100</f>
-        <v>-6.1489278867575043</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>9.5206529999999994</v>
-      </c>
-      <c r="C6">
-        <v>10.260292750000001</v>
-      </c>
-      <c r="D6" s="21">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <f>B10-B11</f>
-        <v>-1.4934899999999995</v>
-      </c>
-      <c r="F6">
-        <f>(B10-B11)/B11*100</f>
-        <v>-13.674275389023604</v>
-      </c>
-      <c r="G6">
-        <f>C10-C11</f>
-        <v>-2.1598272500000011</v>
-      </c>
-      <c r="H6">
-        <f>(C10-C11)/C11*100</f>
-        <v>-19.701614790491924</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>9.8293160000000004</v>
-      </c>
-      <c r="C7">
-        <v>10.952586750000002</v>
-      </c>
-      <c r="D7" s="21">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <f>B12-B13</f>
-        <v>-0.16019100000000108</v>
-      </c>
-      <c r="F7">
-        <f>(B12-B13)/B13*100</f>
-        <v>-1.6788012811168269</v>
-      </c>
-      <c r="G7">
-        <f>C12-C13</f>
-        <v>0.85087324999999936</v>
-      </c>
-      <c r="H7">
-        <f>(C12-C13)/C13*100</f>
-        <v>8.2566998338346291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>9.1254899999999992</v>
-      </c>
-      <c r="C8">
-        <v>9.7877445000000005</v>
-      </c>
-      <c r="D8" s="21">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <f>B14-B15</f>
-        <v>-0.9318919999999995</v>
-      </c>
-      <c r="F8">
-        <f>(B14-B15)/B15*100</f>
-        <v>-9.058404806954389</v>
-      </c>
-      <c r="G8">
-        <f>C14-C15</f>
-        <v>-0.79258325000000163</v>
-      </c>
-      <c r="H8">
-        <f>(C14-C15)/C15*100</f>
-        <v>-7.7274152716978657</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>9.0093949999999996</v>
-      </c>
-      <c r="C9">
-        <v>10.429017250000001</v>
-      </c>
-      <c r="D9" s="21">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <f>B16-B17</f>
-        <v>-1.2936880000000013</v>
-      </c>
-      <c r="F9">
-        <f>(B16-B17)/B17*100</f>
-        <v>-11.64474843707611</v>
-      </c>
-      <c r="G9">
-        <f>C16-C17</f>
-        <v>-1.4686440000000012</v>
-      </c>
-      <c r="H9">
-        <f>(C16-C17)/C17*100</f>
-        <v>-12.682308661961972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>9.4284049999999997</v>
-      </c>
-      <c r="C10">
-        <v>8.8028642500000007</v>
-      </c>
-      <c r="D10" s="21">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <f>B18-B19</f>
-        <v>-1.0437729999999998</v>
-      </c>
-      <c r="F10">
-        <f>(B18-B19)/B19*100</f>
-        <v>-8.4879916370220343</v>
-      </c>
-      <c r="G10">
-        <f>C18-C19</f>
-        <v>-1.0508347499999982</v>
-      </c>
-      <c r="H10">
-        <f>(C18-C19)/C19*100</f>
-        <v>-8.4730079257860496</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>10.921894999999999</v>
-      </c>
-      <c r="C11">
-        <v>10.962691500000002</v>
-      </c>
-      <c r="D11" s="21">
-        <v>13</v>
-      </c>
-      <c r="E11">
-        <f>B20-B21</f>
-        <v>-0.82010000000000005</v>
-      </c>
-      <c r="F11">
-        <f>(B20-B21)/B21*100</f>
-        <v>-7.4979090698643125</v>
-      </c>
-      <c r="G11">
-        <f>C20-C21</f>
-        <v>-2.3854830000000007</v>
-      </c>
-      <c r="H11">
-        <f>(C20-C21)/C21*100</f>
-        <v>-17.909158925886505</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>9.3817959999999996</v>
-      </c>
-      <c r="C12">
-        <v>11.156119500000001</v>
-      </c>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>9.5419870000000007</v>
-      </c>
-      <c r="C13">
-        <v>10.305246250000001</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="H13" s="36" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>9.3557030000000001</v>
-      </c>
-      <c r="C14">
-        <v>9.4641872500000002</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36">
-        <f>AVERAGE(E2:E11)</f>
-        <v>-0.65684070000000028</v>
-      </c>
-      <c r="F14" s="36">
-        <f>AVERAGE(F2:F11)</f>
-        <v>-6.0248504540741381</v>
-      </c>
-      <c r="G14" s="36">
-        <f>AVERAGE(G2:G11)</f>
-        <v>-1.0781909000000005</v>
-      </c>
-      <c r="H14" s="36">
-        <f>AVERAGE(H2:H11)</f>
-        <v>-9.2415870532644497</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>10.287595</v>
-      </c>
-      <c r="C15">
-        <v>10.256770500000002</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="H15" s="36" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>9.8159379999999992</v>
-      </c>
-      <c r="C16">
-        <v>10.111613500000001</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="36">
-        <f>_xlfn.STDEV.P(E2:E11)</f>
-        <v>0.50747297712490058</v>
-      </c>
-      <c r="F16" s="36">
-        <f>_xlfn.STDEV.P(F2:F11)</f>
-        <v>4.5571426681842135</v>
-      </c>
-      <c r="G16" s="36">
-        <f>_xlfn.STDEV.P(G2:G11)</f>
-        <v>0.8502260917791824</v>
-      </c>
-      <c r="H16" s="36">
-        <f>_xlfn.STDEV.P(H2:H11)</f>
-        <v>7.2716637751868829</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>11.109626</v>
-      </c>
-      <c r="C17">
-        <v>11.580257500000002</v>
-      </c>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18">
-        <v>11.253282</v>
-      </c>
-      <c r="C18">
-        <v>11.351310500000002</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>10</v>
-      </c>
-      <c r="B19">
-        <v>12.297055</v>
-      </c>
-      <c r="C19">
-        <v>12.40214525</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="27">
-        <f>AVERAGE(E3:E4,E6,E8:E11)</f>
-        <v>-0.90132342857142866</v>
-      </c>
-      <c r="F19" s="27">
-        <f>AVERAGE(F3:F4,F6,F8:F11)</f>
-        <v>-8.2787415045902168</v>
-      </c>
-      <c r="G19" s="27">
-        <f>AVERAGE(G3:G4,G6,G8:G11)</f>
-        <v>-1.4074365357142862</v>
-      </c>
-      <c r="H19" s="27">
-        <f>AVERAGE(H3:H4,H6,H8:H11)</f>
-        <v>-11.967196031318531</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="B20">
-        <v>10.117616</v>
-      </c>
-      <c r="C20">
-        <v>10.934422250000001</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>13</v>
-      </c>
-      <c r="B21">
-        <v>10.937716</v>
-      </c>
-      <c r="C21">
-        <v>13.319905250000001</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="27">
-        <f>_xlfn.STDEV.P(E3:E4,E6,E8:E11)</f>
-        <v>0.39957359395945252</v>
-      </c>
-      <c r="F21" s="27">
-        <f>_xlfn.STDEV.P(F3:F4,F6,F8:F11)</f>
-        <v>3.4389545442921081</v>
-      </c>
-      <c r="G21" s="27">
-        <f>_xlfn.STDEV.P(G3:G4,G6,G8:G11)</f>
-        <v>0.60404424501591514</v>
-      </c>
-      <c r="H21" s="27">
-        <f>_xlfn.STDEV.P(H3:H4,H6,H8:H11)</f>
-        <v>4.7618807758293462</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E23">
-        <f>E21/SQRT(COUNT(E8:E11,E6,E3:E4))</f>
-        <v>0.15102462286928742</v>
-      </c>
-      <c r="F23">
-        <f>F21/SQRT(COUNT(F8:F11,F6,F3:F4))</f>
-        <v>1.2998026420360538</v>
-      </c>
-      <c r="G23">
-        <f>G21/SQRT(COUNT(G8:G11,G6,G3:G4))</f>
-        <v>0.22830726474169688</v>
-      </c>
-      <c r="H23">
-        <f>H21/SQRT(COUNT(H8:H11,H6,H3:H4))</f>
-        <v>1.7998217579691089</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="G26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>214</v>
-      </c>
-      <c r="C27" t="s">
-        <v>215</v>
-      </c>
-      <c r="D27" t="s">
-        <v>216</v>
-      </c>
-      <c r="E27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>9.3905689999999993</v>
-      </c>
-      <c r="C28">
-        <v>8.9729109999999999</v>
-      </c>
-      <c r="D28">
-        <v>11.887410750000001</v>
-      </c>
-      <c r="E28">
-        <v>10.58502125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>9.8293160000000004</v>
-      </c>
-      <c r="C29">
-        <v>9.5206529999999994</v>
-      </c>
-      <c r="D29">
-        <v>10.952586750000002</v>
-      </c>
-      <c r="E29">
-        <v>10.260292750000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>10.921894999999999</v>
-      </c>
-      <c r="C30">
-        <v>9.4284049999999997</v>
-      </c>
-      <c r="D30">
-        <v>10.962691500000002</v>
-      </c>
-      <c r="E30">
-        <v>8.8028642500000007</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>10.287595</v>
-      </c>
-      <c r="C31">
-        <v>9.3557030000000001</v>
-      </c>
-      <c r="D31">
-        <v>10.256770500000002</v>
-      </c>
-      <c r="E31">
-        <v>9.4641872500000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>11.109626</v>
-      </c>
-      <c r="C32">
-        <v>9.8159379999999992</v>
-      </c>
-      <c r="D32">
-        <v>11.580257500000002</v>
-      </c>
-      <c r="E32">
-        <v>10.111613500000001</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>12.297055</v>
-      </c>
-      <c r="C33">
-        <v>11.253282</v>
-      </c>
-      <c r="D33">
-        <v>12.40214525</v>
-      </c>
-      <c r="E33">
-        <v>11.351310500000002</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>10.937716</v>
-      </c>
-      <c r="C34">
-        <v>10.117616</v>
-      </c>
-      <c r="D34">
-        <v>13.319905250000001</v>
-      </c>
-      <c r="E34">
-        <v>10.934422250000001</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>219</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E41" s="21"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>10.681967428571427</v>
-      </c>
-      <c r="D43">
-        <v>9.7806439999999988</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43">
-        <v>11.623109642857145</v>
-      </c>
-      <c r="G43">
-        <v>10.215673107142859</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44">
-        <v>0.91077104346628623</v>
-      </c>
-      <c r="D44">
-        <v>0.55135559337266693</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44">
-        <v>1.0517231529273505</v>
-      </c>
-      <c r="G44">
-        <v>0.75271164061995599</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45">
-        <v>7</v>
-      </c>
-      <c r="D45">
-        <v>7</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45">
-        <v>7</v>
-      </c>
-      <c r="G45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46">
-        <v>0.90022642372726802</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46">
-        <v>0.77480369522652626</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48">
-        <v>6</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49">
-        <v>5.5253463356738246</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49">
-        <v>5.7073656214696671</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50">
-        <v>7.397762964505794E-4</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50">
-        <v>6.2590716172419164E-4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51">
-        <v>1.9431802805153031</v>
-      </c>
-      <c r="E51" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51">
-        <v>1.9431802805153031</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52">
-        <v>1.4795525929011588E-3</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52">
-        <v>1.2518143234483833E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="1">
-        <v>2.4469118511449697</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="1">
-        <v>2.4469118511449697</v>
-      </c>
-      <c r="G53" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reran some sims with higher convergence tolerances and with higher weights on the effort term. Did not see large differences.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons_rev2.xlsx
+++ b/metaboliccostcomparisons_rev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C856C-943D-4246-A9E7-3207CEF5FDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7454DB67-3E7A-4CB7-BFCA-0D836F04F362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="573" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="573" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fullcost t test" sheetId="5" r:id="rId1"/>
@@ -2859,21 +2859,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -2957,21 +2942,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -3772,22 +3742,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
+                  <a:defRPr b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US" b="0"/>
                   <a:t>Simulated Cost (W/kg)</a:t>
                 </a:r>
               </a:p>
@@ -3808,27 +3766,11 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="BFBFBF"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="64009006"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -3858,22 +3800,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
+                  <a:defRPr b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US" b="0"/>
                   <a:t>Measured Cost (W/kg)</a:t>
                 </a:r>
               </a:p>
@@ -3902,27 +3832,11 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="BFBFBF"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="67023442"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -3944,17 +3858,15 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
+              <a:defRPr sz="2800" b="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
         <c:idx val="8"/>
@@ -3982,13 +3894,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
+            <a:defRPr sz="2800" b="0"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -4009,6 +3915,22 @@
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="3200">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -48619,8 +48541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA391E9-48A1-41F4-999A-C126E3EDA00F}">
   <dimension ref="A1:CR141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="E71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added all of the statistics from all the plotting scripts - these were reprocessed for the new prediction project.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons_rev2.xlsx
+++ b/metaboliccostcomparisons_rev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonstingel\code\musclemodel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7454DB67-3E7A-4CB7-BFCA-0D836F04F362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4472ECFF-E210-41DF-BAB9-FF7EEAB58CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="573" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="2376" windowWidth="14028" windowHeight="8832" tabRatio="803" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fullcost t test" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="231">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -728,6 +728,12 @@
   </si>
   <si>
     <t>std ones that we want</t>
+  </si>
+  <si>
+    <t>std natural</t>
+  </si>
+  <si>
+    <t>std exo</t>
   </si>
 </sst>
 </file>
@@ -44727,9 +44733,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -44767,7 +44773,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -44873,7 +44879,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -45015,7 +45021,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -45025,8 +45031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45424,7 +45430,7 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45811,6 +45817,12 @@
       <c r="B14">
         <v>3.7305519239537739E-2</v>
       </c>
+      <c r="K14" t="s">
+        <v>230</v>
+      </c>
+      <c r="L14" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -45823,6 +45835,14 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
+      <c r="K15">
+        <f>_xlfn.STDEV.P(K3:K9)</f>
+        <v>0.3362888641794462</v>
+      </c>
+      <c r="L15">
+        <f>_xlfn.STDEV.P(O3:O9)</f>
+        <v>0.46933820097839557</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I16" s="10" t="s">
@@ -46920,6 +46940,22 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
+      <c r="N15" t="s">
+        <v>229</v>
+      </c>
+      <c r="O15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <f>_xlfn.STDEV.P(N3:N9)</f>
+        <v>1.0478874352242364</v>
+      </c>
+      <c r="O16">
+        <f>_xlfn.STDEV.P(R3:R9)</f>
+        <v>1.0505865455651497</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -47609,8 +47645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1ABE7E-150E-4D46-958B-4C378FF29328}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48209,7 +48245,6 @@
       <c r="B26" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -48295,7 +48330,7 @@
         <v>10.111613500000001</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>12.297055</v>
       </c>
@@ -48309,7 +48344,7 @@
         <v>11.351310500000002</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>10.937716</v>
       </c>
@@ -48323,7 +48358,54 @@
         <v>10.934422250000001</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35">
+        <f>AVERAGE(B28:B34)</f>
+        <v>10.681967428571427</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:E35" si="0">AVERAGE(C28:C34)</f>
+        <v>9.7806439999999988</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>11.623109642857145</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>10.215673107142859</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36">
+        <f>_xlfn.STDEV.P(B28:B34)</f>
+        <v>0.88355016518569784</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:E36" si="1">_xlfn.STDEV.P(C28:C34)</f>
+        <v>0.68745218641382111</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>0.94946142008163936</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>0.80323185086603521</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>219</v>
       </c>
@@ -48331,7 +48413,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -48339,10 +48421,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E41" s="21"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
         <v>1</v>
@@ -48358,7 +48440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>3</v>
       </c>
@@ -48378,7 +48460,7 @@
         <v>10.215673107142859</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>4</v>
       </c>
@@ -48398,7 +48480,7 @@
         <v>0.75271164061995599</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>6</v>
       </c>
@@ -48418,7 +48500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>7</v>
       </c>
@@ -48432,7 +48514,7 @@
         <v>0.77480369522652626</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>5</v>
       </c>
@@ -48446,7 +48528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>8</v>
       </c>
@@ -48541,8 +48623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA391E9-48A1-41F4-999A-C126E3EDA00F}">
   <dimension ref="A1:CR141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -59181,7 +59263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:CP81"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>

</xml_diff>